<commit_message>
Aggiunta voce DEVICES > OTHER > BOILER per indicare se il bollitore è da 400cc o da 800cc Un po' di refactoring del codice e aggiunta di tanti commenti
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="435" windowWidth="24765" windowHeight="14070" activeTab="8"/>
+    <workbookView xWindow="3120" yWindow="435" windowWidth="24765" windowHeight="14070"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="987">
   <si>
     <t>LABEL</t>
   </si>
@@ -2991,6 +2991,9 @@
   </si>
   <si>
     <t>TEMPS DE DISSOLUTION PASTEL</t>
+  </si>
+  <si>
+    <t>$LAB_BOILER</t>
   </si>
 </sst>
 </file>
@@ -3317,7 +3320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3325,10 +3328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4182,6 +4185,20 @@
       </c>
       <c r="D62" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>986</v>
+      </c>
+      <c r="B63" t="s">
+        <v>332</v>
+      </c>
+      <c r="C63" t="s">
+        <v>333</v>
+      </c>
+      <c r="D63" t="s">
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -7238,7 +7255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modificata gestione menu Milker in menu prog. Il btn MILKER è sempre attivo, anche se CPU riporta che il milker è scollegato. Aggiunto btn ENABLED YES NO
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rhea\rheaSRC\gpu-fts-nestle-2019\MenuProgTranslator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="6"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -24,8 +29,8 @@
     <sheet name="Menu Data Audit" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="1435">
   <si>
     <t>LABEL</t>
   </si>
@@ -4340,13 +4345,25 @@
   </si>
   <si>
     <t>CONTATORE</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER_VERSION</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>VERSIONE</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER_STATUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4420,7 +4437,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4690,21 +4707,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
@@ -4714,7 +4731,7 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4734,7 +4751,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
@@ -4754,7 +4771,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -4774,7 +4791,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>553</v>
       </c>
@@ -4788,7 +4805,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>384</v>
       </c>
@@ -4808,7 +4825,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>158</v>
       </c>
@@ -4828,7 +4845,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -4848,7 +4865,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>538</v>
       </c>
@@ -4868,7 +4885,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>915</v>
       </c>
@@ -4888,7 +4905,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -4908,7 +4925,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>135</v>
       </c>
@@ -4928,7 +4945,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>529</v>
       </c>
@@ -4948,7 +4965,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -4968,7 +4985,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>331</v>
       </c>
@@ -4985,7 +5002,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>214</v>
       </c>
@@ -5005,7 +5022,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>400</v>
       </c>
@@ -5025,7 +5042,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -5042,7 +5059,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>719</v>
       </c>
@@ -5062,7 +5079,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>217</v>
       </c>
@@ -5082,7 +5099,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>605</v>
       </c>
@@ -5102,7 +5119,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>502</v>
       </c>
@@ -5122,7 +5139,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -5142,7 +5159,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -5162,7 +5179,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>129</v>
       </c>
@@ -5182,7 +5199,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>536</v>
       </c>
@@ -5202,7 +5219,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>706</v>
       </c>
@@ -5220,7 +5237,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>142</v>
       </c>
@@ -5240,7 +5257,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>345</v>
       </c>
@@ -5260,7 +5277,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
@@ -5280,7 +5297,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>132</v>
       </c>
@@ -5300,7 +5317,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>602</v>
       </c>
@@ -5320,7 +5337,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>188</v>
       </c>
@@ -5340,7 +5357,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>138</v>
       </c>
@@ -5360,7 +5377,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>526</v>
       </c>
@@ -5380,7 +5397,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>144</v>
       </c>
@@ -5397,7 +5414,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>109</v>
       </c>
@@ -5417,7 +5434,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>177</v>
       </c>
@@ -5437,7 +5454,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -5457,7 +5474,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>221</v>
       </c>
@@ -5477,7 +5494,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>390</v>
       </c>
@@ -5497,7 +5514,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>566</v>
       </c>
@@ -5517,7 +5534,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>49</v>
       </c>
@@ -5528,7 +5545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
@@ -5548,7 +5565,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>594</v>
       </c>
@@ -5568,7 +5585,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>503</v>
       </c>
@@ -5588,7 +5605,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -5608,7 +5625,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>533</v>
       </c>
@@ -5628,7 +5645,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>198</v>
       </c>
@@ -5648,7 +5665,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>704</v>
       </c>
@@ -5668,7 +5685,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>185</v>
       </c>
@@ -5688,7 +5705,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>148</v>
       </c>
@@ -5708,7 +5725,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>506</v>
       </c>
@@ -5728,7 +5745,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>211</v>
       </c>
@@ -5748,7 +5765,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>98</v>
       </c>
@@ -5768,7 +5785,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>499</v>
       </c>
@@ -5788,7 +5805,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>492</v>
       </c>
@@ -5808,7 +5825,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -5828,7 +5845,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>189</v>
       </c>
@@ -5848,7 +5865,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
@@ -5868,7 +5885,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>495</v>
       </c>
@@ -5888,7 +5905,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>36</v>
       </c>
@@ -5908,7 +5925,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>947</v>
       </c>
@@ -5922,7 +5939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>970</v>
       </c>
@@ -5936,7 +5953,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1428</v>
       </c>
@@ -5957,14 +5974,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -5974,7 +5991,7 @@
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5994,7 +6011,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -6011,7 +6028,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -6028,7 +6045,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -6045,7 +6062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -6065,7 +6082,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -6085,7 +6102,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -6105,7 +6122,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -6122,7 +6139,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -6142,7 +6159,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -6162,7 +6179,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -6179,7 +6196,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -6199,7 +6216,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -6219,7 +6236,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -6239,7 +6256,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>732</v>
       </c>
@@ -6259,7 +6276,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>731</v>
       </c>
@@ -6279,7 +6296,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>728</v>
       </c>
@@ -6299,7 +6316,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>729</v>
       </c>
@@ -6319,7 +6336,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -6339,7 +6356,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>194</v>
       </c>
@@ -6359,7 +6376,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>245</v>
       </c>
@@ -6379,7 +6396,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>250</v>
       </c>
@@ -6399,7 +6416,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>249</v>
       </c>
@@ -6419,7 +6436,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>256</v>
       </c>
@@ -6439,7 +6456,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>257</v>
       </c>
@@ -6459,7 +6476,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>260</v>
       </c>
@@ -6479,7 +6496,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>261</v>
       </c>
@@ -6490,7 +6507,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>263</v>
       </c>
@@ -6510,7 +6527,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>265</v>
       </c>
@@ -6530,7 +6547,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>269</v>
       </c>
@@ -6550,7 +6567,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>618</v>
       </c>
@@ -6570,7 +6587,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>620</v>
       </c>
@@ -6590,7 +6607,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>622</v>
       </c>
@@ -6617,14 +6634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -6634,7 +6651,7 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6654,7 +6671,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>270</v>
       </c>
@@ -6674,7 +6691,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>277</v>
       </c>
@@ -6694,7 +6711,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>275</v>
       </c>
@@ -6714,7 +6731,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -6731,7 +6748,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>314</v>
       </c>
@@ -6751,7 +6768,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -6771,7 +6788,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>284</v>
       </c>
@@ -6791,7 +6808,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>287</v>
       </c>
@@ -6811,7 +6828,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>289</v>
       </c>
@@ -6831,7 +6848,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>292</v>
       </c>
@@ -6851,7 +6868,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>297</v>
       </c>
@@ -6871,7 +6888,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -6891,7 +6908,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>304</v>
       </c>
@@ -6911,7 +6928,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>307</v>
       </c>
@@ -6931,7 +6948,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>310</v>
       </c>
@@ -6951,7 +6968,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>311</v>
       </c>
@@ -6971,7 +6988,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>599</v>
       </c>
@@ -6991,7 +7008,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>702</v>
       </c>
@@ -7002,7 +7019,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>905</v>
       </c>
@@ -7019,7 +7036,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>906</v>
       </c>
@@ -7036,7 +7053,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>909</v>
       </c>
@@ -7056,7 +7073,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>911</v>
       </c>
@@ -7076,7 +7093,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>919</v>
       </c>
@@ -7103,14 +7120,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
@@ -7119,7 +7136,7 @@
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7139,7 +7156,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>316</v>
       </c>
@@ -7159,7 +7176,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>323</v>
       </c>
@@ -7179,7 +7196,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>322</v>
       </c>
@@ -7199,7 +7216,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -7219,7 +7236,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>597</v>
       </c>
@@ -7245,14 +7262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -7262,7 +7279,7 @@
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7282,7 +7299,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>330</v>
       </c>
@@ -7302,7 +7319,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>335</v>
       </c>
@@ -7322,7 +7339,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>338</v>
       </c>
@@ -7342,7 +7359,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>341</v>
       </c>
@@ -7368,14 +7385,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" customWidth="1"/>
@@ -7385,7 +7402,7 @@
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -7405,7 +7422,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>347</v>
       </c>
@@ -7423,7 +7440,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>351</v>
       </c>
@@ -7441,7 +7458,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>355</v>
       </c>
@@ -7461,7 +7478,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>356</v>
       </c>
@@ -7481,7 +7498,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>357</v>
       </c>
@@ -7495,7 +7512,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>361</v>
       </c>
@@ -7515,7 +7532,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>365</v>
       </c>
@@ -7533,7 +7550,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>367</v>
       </c>
@@ -7553,7 +7570,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>368</v>
       </c>
@@ -7573,7 +7590,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>373</v>
       </c>
@@ -7591,7 +7608,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>376</v>
       </c>
@@ -7611,7 +7628,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>380</v>
       </c>
@@ -7629,7 +7646,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>382</v>
       </c>
@@ -7649,7 +7666,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>389</v>
       </c>
@@ -7669,7 +7686,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>394</v>
       </c>
@@ -7689,7 +7706,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>397</v>
       </c>
@@ -7709,7 +7726,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>742</v>
       </c>
@@ -7729,7 +7746,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>745</v>
       </c>
@@ -7755,14 +7772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
@@ -7772,7 +7789,7 @@
     <col min="6" max="6" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7792,7 +7809,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -7812,7 +7829,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>227</v>
       </c>
@@ -7832,7 +7849,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -7852,7 +7869,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>237</v>
       </c>
@@ -7872,7 +7889,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>236</v>
       </c>
@@ -7889,7 +7906,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -7915,14 +7932,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
@@ -7932,7 +7949,7 @@
     <col min="6" max="6" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7952,7 +7969,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>542</v>
       </c>
@@ -7972,7 +7989,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>543</v>
       </c>
@@ -7992,7 +8009,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>545</v>
       </c>
@@ -8012,7 +8029,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>548</v>
       </c>
@@ -8032,7 +8049,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>551</v>
       </c>
@@ -8052,7 +8069,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>555</v>
       </c>
@@ -8072,7 +8089,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>560</v>
       </c>
@@ -8092,7 +8109,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -8100,7 +8117,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>563</v>
       </c>
@@ -8120,7 +8137,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>565</v>
       </c>
@@ -8140,7 +8157,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -8148,7 +8165,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>572</v>
       </c>
@@ -8168,7 +8185,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -8176,7 +8193,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="45">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>574</v>
       </c>
@@ -8196,7 +8213,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>576</v>
       </c>
@@ -8216,7 +8233,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>579</v>
       </c>
@@ -8236,7 +8253,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="75">
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>581</v>
       </c>
@@ -8256,7 +8273,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>583</v>
       </c>
@@ -8276,7 +8293,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>585</v>
       </c>
@@ -8296,7 +8313,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -8304,7 +8321,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>587</v>
       </c>
@@ -8324,7 +8341,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>591</v>
       </c>
@@ -8344,7 +8361,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -8352,7 +8369,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="105">
+    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>735</v>
       </c>
@@ -8379,14 +8396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.140625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -8394,7 +8411,7 @@
     <col min="6" max="6" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8414,7 +8431,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>687</v>
       </c>
@@ -8434,7 +8451,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>688</v>
       </c>
@@ -8454,7 +8471,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>689</v>
       </c>
@@ -8465,7 +8482,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>690</v>
       </c>
@@ -8485,7 +8502,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>711</v>
       </c>
@@ -8505,7 +8522,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>714</v>
       </c>
@@ -8525,7 +8542,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>691</v>
       </c>
@@ -8545,7 +8562,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>692</v>
       </c>
@@ -8565,7 +8582,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>693</v>
       </c>
@@ -8585,7 +8602,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75">
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>694</v>
       </c>
@@ -8605,7 +8622,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>695</v>
       </c>
@@ -8625,7 +8642,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>696</v>
       </c>
@@ -8645,7 +8662,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>697</v>
       </c>
@@ -8665,7 +8682,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>698</v>
       </c>
@@ -8685,7 +8702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>699</v>
       </c>
@@ -8705,7 +8722,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
   </sheetData>
@@ -8715,14 +8732,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="36.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="36.7109375" style="6"/>
     <col min="5" max="5" width="16.85546875" style="6" customWidth="1"/>
@@ -8730,7 +8747,7 @@
     <col min="7" max="16384" width="36.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -8750,7 +8767,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>866</v>
       </c>
@@ -8770,7 +8787,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>869</v>
       </c>
@@ -8790,7 +8807,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>873</v>
       </c>
@@ -8810,7 +8827,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>874</v>
       </c>
@@ -8830,7 +8847,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30.75" customHeight="1">
+    <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>879</v>
       </c>
@@ -8850,7 +8867,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>881</v>
       </c>
@@ -8870,7 +8887,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>883</v>
       </c>
@@ -8890,7 +8907,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>894</v>
       </c>
@@ -8910,7 +8927,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>898</v>
       </c>
@@ -8930,7 +8947,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>924</v>
       </c>
@@ -8950,7 +8967,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>925</v>
       </c>
@@ -8970,7 +8987,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>926</v>
       </c>
@@ -8996,14 +9013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
@@ -9013,7 +9030,7 @@
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -9033,7 +9050,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>200</v>
       </c>
@@ -9053,7 +9070,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>201</v>
       </c>
@@ -9073,7 +9090,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>202</v>
       </c>
@@ -9093,7 +9110,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>203</v>
       </c>
@@ -9113,7 +9130,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>204</v>
       </c>
@@ -9133,7 +9150,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>205</v>
       </c>
@@ -9153,7 +9170,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>206</v>
       </c>
@@ -9173,7 +9190,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>207</v>
       </c>
@@ -9193,7 +9210,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>208</v>
       </c>
@@ -9213,7 +9230,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>210</v>
       </c>
@@ -9233,7 +9250,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>209</v>
       </c>
@@ -9259,14 +9276,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" style="6" customWidth="1"/>
@@ -9277,7 +9292,7 @@
     <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -9297,7 +9312,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>511</v>
       </c>
@@ -9317,7 +9332,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>513</v>
       </c>
@@ -9337,7 +9352,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>515</v>
       </c>
@@ -9357,7 +9372,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>517</v>
       </c>
@@ -9377,7 +9392,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>520</v>
       </c>
@@ -9397,7 +9412,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>521</v>
       </c>
@@ -9414,7 +9429,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>523</v>
       </c>
@@ -9434,7 +9449,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>525</v>
       </c>
@@ -9454,7 +9469,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>709</v>
       </c>
@@ -9474,8 +9489,30 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="10"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9484,14 +9521,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" customWidth="1"/>
@@ -9499,7 +9536,7 @@
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -9519,7 +9556,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>402</v>
       </c>
@@ -9539,7 +9576,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>407</v>
       </c>
@@ -9559,7 +9596,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>409</v>
       </c>
@@ -9579,7 +9616,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>413</v>
       </c>
@@ -9599,7 +9636,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>416</v>
       </c>
@@ -9619,7 +9656,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>419</v>
       </c>
@@ -9639,7 +9676,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>421</v>
       </c>
@@ -9657,7 +9694,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>424</v>
       </c>
@@ -9675,7 +9712,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>428</v>
       </c>
@@ -9693,7 +9730,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>430</v>
       </c>
@@ -9713,7 +9750,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>433</v>
       </c>
@@ -9733,7 +9770,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>435</v>
       </c>
@@ -9751,7 +9788,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>438</v>
       </c>
@@ -9771,7 +9808,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>440</v>
       </c>
@@ -9791,7 +9828,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>443</v>
       </c>
@@ -9811,7 +9848,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>446</v>
       </c>
@@ -9831,7 +9868,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>449</v>
       </c>
@@ -9851,7 +9888,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>451</v>
       </c>
@@ -9871,7 +9908,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>458</v>
       </c>
@@ -9891,7 +9928,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>934</v>
       </c>
@@ -9907,7 +9944,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>937</v>
       </c>
@@ -9923,7 +9960,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>939</v>
       </c>
@@ -9935,7 +9972,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>941</v>
       </c>
@@ -9951,7 +9988,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>944</v>
       </c>
@@ -9967,7 +10004,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>948</v>
       </c>
@@ -9983,7 +10020,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>954</v>
       </c>
@@ -10008,14 +10045,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
@@ -10024,7 +10061,7 @@
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10044,7 +10081,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>460</v>
       </c>
@@ -10064,7 +10101,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>461</v>
       </c>
@@ -10084,7 +10121,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>465</v>
       </c>
@@ -10104,7 +10141,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>468</v>
       </c>
@@ -10124,7 +10161,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>470</v>
       </c>
@@ -10144,7 +10181,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>471</v>
       </c>
@@ -10164,7 +10201,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>476</v>
       </c>
@@ -10184,7 +10221,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>479</v>
       </c>
@@ -10204,7 +10241,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>482</v>
       </c>
@@ -10224,7 +10261,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>484</v>
       </c>
@@ -10250,14 +10287,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
@@ -10266,7 +10303,7 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10286,7 +10323,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -10306,7 +10343,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -10326,7 +10363,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -10346,7 +10383,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -10366,7 +10403,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -10386,7 +10423,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -10406,7 +10443,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -10426,7 +10463,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -10446,7 +10483,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -10466,7 +10503,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>963</v>
       </c>
@@ -10480,7 +10517,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>965</v>
       </c>

</xml_diff>

<commit_message>
Aggiunta funzionalità in menu prog DEVICES > MICRO > GRINDER SPEED FOR OFF 09 Si attiva solo se la macchina è multibona e il gruppo è micro
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="1696">
   <si>
     <t>LABEL</t>
   </si>
@@ -5134,6 +5134,12 @@
   </si>
   <si>
     <t>没有</t>
+  </si>
+  <si>
+    <t>$LAB_DEV_GRINDER_SPEED_FOR_OFF09</t>
+  </si>
+  <si>
+    <t>GRINDER SPEED FOR OFF09</t>
   </si>
 </sst>
 </file>
@@ -5560,8 +5566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5730,1286 +5736,1286 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>538</v>
+        <v>970</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>326</v>
       </c>
       <c r="C8" t="s">
-        <v>540</v>
+        <v>327</v>
       </c>
       <c r="D8" t="s">
-        <v>615</v>
-      </c>
-      <c r="E8" t="s">
-        <v>989</v>
-      </c>
-      <c r="F8" t="s">
-        <v>990</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>1455</v>
+        <v>843</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
       <c r="A9" t="s">
+        <v>538</v>
+      </c>
+      <c r="B9" t="s">
+        <v>539</v>
+      </c>
+      <c r="C9" t="s">
+        <v>540</v>
+      </c>
+      <c r="D9" t="s">
+        <v>615</v>
+      </c>
+      <c r="E9" t="s">
+        <v>989</v>
+      </c>
+      <c r="F9" t="s">
+        <v>990</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75">
+      <c r="A10" t="s">
         <v>915</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>136</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>916</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>917</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>991</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>992</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>1456</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" t="s">
-        <v>616</v>
-      </c>
-      <c r="E10" t="s">
-        <v>993</v>
-      </c>
-      <c r="F10" t="s">
-        <v>993</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>1457</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="3" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>994</v>
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>616</v>
+      </c>
+      <c r="E11" t="s">
+        <v>993</v>
       </c>
       <c r="F11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="F12" t="s">
+        <v>992</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
+      <c r="A13" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>530</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>531</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>995</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>1458</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>632</v>
-      </c>
-      <c r="E13" t="s">
-        <v>996</v>
-      </c>
-      <c r="F13" t="s">
-        <v>997</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>1459</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>331</v>
+        <v>1439</v>
       </c>
       <c r="B14" t="s">
-        <v>332</v>
+        <v>1440</v>
       </c>
       <c r="C14" t="s">
-        <v>333</v>
-      </c>
-      <c r="E14" t="s">
-        <v>998</v>
-      </c>
-      <c r="F14" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>1428</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>1429</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" t="s">
-        <v>633</v>
-      </c>
-      <c r="E15" t="s">
-        <v>999</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1000</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>1460</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75">
       <c r="A16" t="s">
-        <v>400</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>399</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>401</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E16" t="s">
-        <v>1001</v>
+        <v>996</v>
       </c>
       <c r="F16" t="s">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>331</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="E17" t="s">
-        <v>1003</v>
+        <v>998</v>
       </c>
       <c r="F17" t="s">
-        <v>1004</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>1462</v>
+        <v>998</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75">
       <c r="A18" t="s">
-        <v>719</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
-        <v>720</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>721</v>
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>722</v>
+        <v>633</v>
       </c>
       <c r="E18" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="F18" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>400</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>399</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>401</v>
       </c>
       <c r="D19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E19" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="F19" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75">
       <c r="A20" t="s">
-        <v>605</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>606</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>607</v>
-      </c>
-      <c r="D20" t="s">
-        <v>636</v>
+        <v>182</v>
       </c>
       <c r="E20" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="F20" t="s">
-        <v>1009</v>
+        <v>1004</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75">
       <c r="A21" t="s">
-        <v>502</v>
+        <v>719</v>
       </c>
       <c r="B21" t="s">
-        <v>500</v>
+        <v>720</v>
       </c>
       <c r="C21" t="s">
-        <v>501</v>
+        <v>721</v>
       </c>
       <c r="D21" t="s">
-        <v>630</v>
+        <v>722</v>
       </c>
       <c r="E21" t="s">
-        <v>1010</v>
+        <v>1005</v>
       </c>
       <c r="F21" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>217</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>219</v>
       </c>
       <c r="D22" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E22" t="s">
-        <v>1012</v>
+        <v>1007</v>
       </c>
       <c r="F22" t="s">
-        <v>1013</v>
+        <v>1008</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75">
       <c r="A23" t="s">
+        <v>605</v>
+      </c>
+      <c r="B23" t="s">
+        <v>606</v>
+      </c>
+      <c r="C23" t="s">
+        <v>607</v>
+      </c>
+      <c r="D23" t="s">
+        <v>636</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75">
+      <c r="A24" t="s">
+        <v>502</v>
+      </c>
+      <c r="B24" t="s">
+        <v>500</v>
+      </c>
+      <c r="C24" t="s">
+        <v>501</v>
+      </c>
+      <c r="D24" t="s">
+        <v>630</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>637</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75">
+      <c r="A26" t="s">
         <v>101</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>29</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>637</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>1014</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>1015</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>1468</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75">
-      <c r="A24" s="3" t="s">
+    <row r="27" spans="1:7" ht="15.75">
+      <c r="A27" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>130</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" t="s">
         <v>1017</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>1469</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75">
-      <c r="A25" s="3" t="s">
+    <row r="28" spans="1:7" ht="15.75">
+      <c r="A28" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>535</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>537</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F28" t="s">
         <v>1019</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>1470</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75">
-      <c r="A26" s="3" t="s">
+    <row r="29" spans="1:7" ht="15.75">
+      <c r="A29" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>707</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>708</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>1020</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>1471</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
-      <c r="A27" t="s">
+    <row r="30" spans="1:7" ht="15.75">
+      <c r="A30" t="s">
         <v>142</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>141</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>143</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>640</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>1022</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>1472</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75">
-      <c r="A28" t="s">
+    <row r="31" spans="1:7" ht="15.75">
+      <c r="A31" t="s">
         <v>345</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>343</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>346</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>641</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>1023</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F31" t="s">
         <v>1024</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>1473</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75">
-      <c r="A29" t="s">
+    <row r="32" spans="1:7" ht="15.75">
+      <c r="A32" t="s">
         <v>488</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>489</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>490</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>629</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>1025</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F32" t="s">
         <v>1026</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G32" s="11" t="s">
         <v>1474</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:7" ht="15.75">
+      <c r="A33" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>133</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>134</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F33" t="s">
         <v>133</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>1475</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75">
-      <c r="A31" s="3" t="s">
-        <v>1692</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1691</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="G31" s="11" t="s">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75">
-      <c r="A32" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="B32" t="s">
-        <v>603</v>
-      </c>
-      <c r="C32" t="s">
-        <v>604</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="F32" t="s">
-        <v>603</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75">
-      <c r="A33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" t="s">
-        <v>187</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1028</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>1477</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="3" t="s">
-        <v>138</v>
+        <v>1692</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1030</v>
-      </c>
+        <v>1691</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
       <c r="G34" s="11" t="s">
-        <v>1478</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="3" t="s">
-        <v>526</v>
+        <v>602</v>
       </c>
       <c r="B35" t="s">
-        <v>527</v>
+        <v>603</v>
       </c>
       <c r="C35" t="s">
-        <v>528</v>
+        <v>604</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1031</v>
+        <v>603</v>
       </c>
       <c r="F35" t="s">
-        <v>1032</v>
+        <v>603</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>187</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>644</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
       <c r="F36" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="3" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="F37" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>1481</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75">
       <c r="A38" s="3" t="s">
-        <v>177</v>
+        <v>526</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>527</v>
       </c>
       <c r="C38" t="s">
-        <v>179</v>
+        <v>528</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="F38" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>1482</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75">
-      <c r="A39" s="3" t="s">
-        <v>103</v>
+      <c r="A39" t="s">
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>648</v>
+        <v>146</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="F39" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75">
       <c r="A40" s="3" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>111</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="F40" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75">
       <c r="A41" s="3" t="s">
-        <v>390</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>391</v>
+        <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>392</v>
+        <v>179</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="F41" t="s">
-        <v>1043</v>
+        <v>1038</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75">
       <c r="A42" s="3" t="s">
-        <v>566</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>567</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>568</v>
+        <v>105</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
       <c r="F42" t="s">
-        <v>1045</v>
+        <v>1040</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75">
       <c r="A43" s="3" t="s">
-        <v>49</v>
+        <v>221</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>220</v>
+      </c>
+      <c r="C43" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>1041</v>
       </c>
       <c r="F43" t="s">
-        <v>50</v>
+        <v>1042</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>390</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>391</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" t="s">
-        <v>723</v>
-      </c>
-      <c r="E44" t="s">
-        <v>1046</v>
+        <v>392</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>1043</v>
       </c>
       <c r="F44" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75">
       <c r="A45" s="3" t="s">
-        <v>594</v>
+        <v>566</v>
       </c>
       <c r="B45" t="s">
-        <v>593</v>
+        <v>567</v>
       </c>
       <c r="C45" t="s">
-        <v>595</v>
+        <v>568</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="F45" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>1488</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75">
       <c r="A46" s="3" t="s">
-        <v>503</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>504</v>
-      </c>
-      <c r="C46" t="s">
-        <v>505</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>1050</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
-        <v>1050</v>
+        <v>50</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75">
-      <c r="A47" t="s">
-        <v>92</v>
+      <c r="A47" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>1051</v>
+        <v>723</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1046</v>
       </c>
       <c r="F47" t="s">
-        <v>1052</v>
+        <v>1047</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>1490</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75">
       <c r="A48" s="3" t="s">
-        <v>533</v>
+        <v>594</v>
       </c>
       <c r="B48" t="s">
-        <v>532</v>
+        <v>593</v>
       </c>
       <c r="C48" t="s">
-        <v>534</v>
+        <v>595</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>1053</v>
+        <v>1048</v>
       </c>
       <c r="F48" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75">
-      <c r="A49" t="s">
-        <v>198</v>
+      <c r="A49" s="3" t="s">
+        <v>503</v>
       </c>
       <c r="B49" t="s">
-        <v>197</v>
+        <v>504</v>
       </c>
       <c r="C49" t="s">
-        <v>199</v>
-      </c>
-      <c r="D49" t="s">
-        <v>655</v>
+        <v>505</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>653</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
       <c r="F49" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>1492</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75">
       <c r="A50" t="s">
-        <v>704</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>477</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>705</v>
+        <v>94</v>
       </c>
       <c r="D50" t="s">
-        <v>748</v>
+        <v>93</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="F50" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>185</v>
+        <v>947</v>
       </c>
       <c r="B51" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>656</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>1059</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>1494</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75">
-      <c r="A52" t="s">
-        <v>148</v>
+      <c r="A52" s="3" t="s">
+        <v>533</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>532</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
-      </c>
-      <c r="D52" t="s">
-        <v>749</v>
+        <v>534</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>654</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>1061</v>
+        <v>1053</v>
       </c>
       <c r="F52" t="s">
-        <v>147</v>
+        <v>1054</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75">
       <c r="A53" t="s">
-        <v>506</v>
+        <v>198</v>
       </c>
       <c r="B53" t="s">
-        <v>507</v>
+        <v>197</v>
       </c>
       <c r="C53" t="s">
-        <v>508</v>
+        <v>199</v>
       </c>
       <c r="D53" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>1062</v>
+        <v>1055</v>
       </c>
       <c r="F53" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>704</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>477</v>
       </c>
       <c r="C54" t="s">
-        <v>213</v>
+        <v>705</v>
       </c>
       <c r="D54" t="s">
-        <v>213</v>
+        <v>748</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>213</v>
+        <v>1057</v>
       </c>
       <c r="F54" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75">
-      <c r="A55" s="3" t="s">
-        <v>98</v>
+      <c r="A55" t="s">
+        <v>185</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>99</v>
+        <v>184</v>
+      </c>
+      <c r="D55" t="s">
+        <v>656</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="F55" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75">
-      <c r="A56" s="3" t="s">
-        <v>499</v>
+      <c r="A56" t="s">
+        <v>148</v>
       </c>
       <c r="B56" t="s">
-        <v>497</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>498</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>658</v>
+        <v>149</v>
+      </c>
+      <c r="D56" t="s">
+        <v>749</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
       <c r="F56" t="s">
-        <v>1067</v>
+        <v>147</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75">
-      <c r="A57" s="3" t="s">
-        <v>492</v>
+      <c r="A57" t="s">
+        <v>506</v>
       </c>
       <c r="B57" t="s">
-        <v>491</v>
+        <v>507</v>
       </c>
       <c r="C57" t="s">
-        <v>493</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>659</v>
+        <v>508</v>
+      </c>
+      <c r="D57" t="s">
+        <v>657</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="F57" t="s">
-        <v>1069</v>
+        <v>1062</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>211</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>660</v>
+        <v>213</v>
+      </c>
+      <c r="D58" t="s">
+        <v>213</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>1070</v>
+        <v>213</v>
       </c>
       <c r="F58" t="s">
-        <v>1071</v>
+        <v>1063</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75">
       <c r="A59" s="3" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>661</v>
+        <v>99</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>1072</v>
+        <v>1064</v>
       </c>
       <c r="F59" t="s">
-        <v>1072</v>
+        <v>1065</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75">
       <c r="A60" s="3" t="s">
-        <v>108</v>
+        <v>499</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>497</v>
       </c>
       <c r="C60" t="s">
-        <v>107</v>
+        <v>498</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>1073</v>
+        <v>1066</v>
       </c>
       <c r="F60" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>1502</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75">
       <c r="A61" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B61" t="s">
+        <v>491</v>
+      </c>
+      <c r="C61" t="s">
+        <v>493</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75">
+      <c r="A63" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75">
+      <c r="A64" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75">
+      <c r="A65" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B65" t="s">
         <v>494</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C65" t="s">
         <v>496</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F65" t="s">
         <v>1075</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G65" s="11" t="s">
         <v>1503</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.75">
-      <c r="A62" s="3" t="s">
+    <row r="66" spans="1:7" ht="15.75">
+      <c r="A66" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B66" t="s">
         <v>37</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C66" t="s">
         <v>38</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D66" t="s">
         <v>609</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F66" t="s">
         <v>1076</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>1504</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>947</v>
-      </c>
-      <c r="B63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>970</v>
-      </c>
-      <c r="B64" t="s">
-        <v>326</v>
-      </c>
-      <c r="C64" t="s">
-        <v>327</v>
-      </c>
-      <c r="D64" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>1428</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1429</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1441</v>
       </c>
     </row>
   </sheetData>
@@ -7783,17 +7789,17 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
@@ -8332,6 +8338,14 @@
       </c>
       <c r="G24" s="19" t="s">
         <v>1659</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunte alcune traduzioni per il menu prog
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="10"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="1711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="1761">
   <si>
     <t>LABEL</t>
   </si>
@@ -5185,6 +5185,156 @@
   </si>
   <si>
     <t>Vel. media con macina vuota</t>
+  </si>
+  <si>
+    <t>Brewer Cleaning is not started (or ended)</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_1</t>
+  </si>
+  <si>
+    <t>Brewer Cleaning is started</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_2</t>
+  </si>
+  <si>
+    <t>Brewer placed</t>
+  </si>
+  <si>
+    <t>Put pastille and push START</t>
+  </si>
+  <si>
+    <t>Infusion</t>
+  </si>
+  <si>
+    <t>Brewer cleaning cycles</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_3</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_4</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_5</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_6</t>
+  </si>
+  <si>
+    <t>Repeat cleaning ?</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_7</t>
+  </si>
+  <si>
+    <t>Brewer placed in brush position, press CONTINUE when finished</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_8</t>
+  </si>
+  <si>
+    <t>Skip final coffee or make a coffee</t>
+  </si>
+  <si>
+    <t>Coffee delivery</t>
+  </si>
+  <si>
+    <t>Rinsing</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_9</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_10</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_11</t>
+  </si>
+  <si>
+    <t>Milker Cleaning is started</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_1</t>
+  </si>
+  <si>
+    <t>Wait for confirm</t>
+  </si>
+  <si>
+    <t>Wait for second confirm</t>
+  </si>
+  <si>
+    <t>Warming for water</t>
+  </si>
+  <si>
+    <t>Warming for cleaner</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_2</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_3</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_4</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_5</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANMILK_6</t>
+  </si>
+  <si>
+    <t>Doing cleaner cycles (12)</t>
+  </si>
+  <si>
+    <t>Lavaggio non iniziato (o terminato)</t>
+  </si>
+  <si>
+    <t>Lavaggio del gruppo in corso</t>
+  </si>
+  <si>
+    <t>Gruppo posizionato</t>
+  </si>
+  <si>
+    <t>Inserire la pastiglia e premere INIZIA</t>
+  </si>
+  <si>
+    <t>Infusione</t>
+  </si>
+  <si>
+    <t>Ciclo di pulizia del gruppo</t>
+  </si>
+  <si>
+    <t>Ripetere la pulizia?</t>
+  </si>
+  <si>
+    <t>Gruppo posizionato, premere CONTINUA quando terminato</t>
+  </si>
+  <si>
+    <t>Si desidera erogare un caffè?</t>
+  </si>
+  <si>
+    <t>Erogazione in corso</t>
+  </si>
+  <si>
+    <t>Risciacquo</t>
+  </si>
+  <si>
+    <t>Lavaggio del cappuccinatore in corso</t>
+  </si>
+  <si>
+    <t>Attesa temperatura</t>
+  </si>
+  <si>
+    <t>Attesa conferma</t>
+  </si>
+  <si>
+    <t>Cicli di lavaggio in corso (12)</t>
+  </si>
+  <si>
+    <t>Attesa seconda conferma</t>
   </si>
 </sst>
 </file>
@@ -7848,7 +7998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -12077,17 +12227,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="43.140625" customWidth="1"/>
@@ -12351,6 +12501,193 @@
         <v>966</v>
       </c>
     </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1760</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nuovi messaggi lavaggio sanitario variflex, passo a linux per compilazione
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -28,7 +28,7 @@
     <sheet name="Payment" sheetId="10" r:id="rId14"/>
     <sheet name="Menu Data Audit" sheetId="6" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="1761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1817">
   <si>
     <t>LABEL</t>
   </si>
@@ -5190,15 +5190,9 @@
     <t>Brewer Cleaning is not started (or ended)</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_1</t>
-  </si>
-  <si>
     <t>Brewer Cleaning is started</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_2</t>
-  </si>
-  <si>
     <t>Brewer placed</t>
   </si>
   <si>
@@ -5211,30 +5205,12 @@
     <t>Brewer cleaning cycles</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_3</t>
-  </si>
-  <si>
-    <t>$LAB_CLEANSAN_4</t>
-  </si>
-  <si>
-    <t>$LAB_CLEANSAN_5</t>
-  </si>
-  <si>
-    <t>$LAB_CLEANSAN_6</t>
-  </si>
-  <si>
     <t>Repeat cleaning ?</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_7</t>
-  </si>
-  <si>
     <t>Brewer placed in brush position, press CONTINUE when finished</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_8</t>
-  </si>
-  <si>
     <t>Skip final coffee or make a coffee</t>
   </si>
   <si>
@@ -5244,15 +5220,6 @@
     <t>Rinsing</t>
   </si>
   <si>
-    <t>$LAB_CLEANSAN_9</t>
-  </si>
-  <si>
-    <t>$LAB_CLEANSAN_10</t>
-  </si>
-  <si>
-    <t>$LAB_CLEANSAN_11</t>
-  </si>
-  <si>
     <t>Milker Cleaning is started</t>
   </si>
   <si>
@@ -5335,6 +5302,207 @@
   </si>
   <si>
     <t>Attesa seconda conferma</t>
+  </si>
+  <si>
+    <t>Cleaning is active</t>
+  </si>
+  <si>
+    <t>Put the pastille in the brewer and press CONTINUE</t>
+  </si>
+  <si>
+    <t>Brewer is closing</t>
+  </si>
+  <si>
+    <t>Tablet dissolution 1/2, please wait</t>
+  </si>
+  <si>
+    <t>2nd dissolution cycle is about to starting</t>
+  </si>
+  <si>
+    <t>Tablet dissolution 2/2, please wait</t>
+  </si>
+  <si>
+    <t>1st Cleaning, please wait</t>
+  </si>
+  <si>
+    <t>1st Cleaning, active 1/3</t>
+  </si>
+  <si>
+    <t>1st Cleaning, active 2/3</t>
+  </si>
+  <si>
+    <t>1st Cleaning, active 3/3</t>
+  </si>
+  <si>
+    <t>Do you want to repeat clean cycle 1/2 ?</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_1</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_2</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_3</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_4</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_5</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_6</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_7</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_8</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_9</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_10</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_MICRO_11</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_0</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_10</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_1</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_2</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_3</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_4</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_5</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_7</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_8</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_9</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_11</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_12</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_13</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_1st_CLEAN_WAIT</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_2nd_CLEAN_WAIT</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, please wait</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 1/6</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 2/6</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 3/6</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 4/6</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 5/6</t>
+  </si>
+  <si>
+    <t>2nd Cleaning, active 6/6</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_14</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_15</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_16</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_17</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_18</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_19</t>
+  </si>
+  <si>
+    <t>Do you want to repeat clean cycle 2/2 ?</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_SKIP_COFFEE</t>
+  </si>
+  <si>
+    <t>LAB_CLEANSAN_VFLEX_20</t>
+  </si>
+  <si>
+    <t>LAB_CLEANSAN_VFLEX_21</t>
+  </si>
+  <si>
+    <t>LAB_CLEANSAN_VFLEX_22</t>
+  </si>
+  <si>
+    <t>LAB_CLEANSAN_VFLEX_23</t>
+  </si>
+  <si>
+    <t>LAB_CLEANSAN_VFLEX_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brewer Rinsing </t>
+  </si>
+  <si>
+    <t>Mixer 1 Rinsing</t>
+  </si>
+  <si>
+    <t>Mixer 2 Rinsing</t>
+  </si>
+  <si>
+    <t>Mixer 3 Rinsing</t>
+  </si>
+  <si>
+    <t>Brewer is going into open position</t>
+  </si>
+  <si>
+    <t>Please, perform a manual brush and then press CONTINUE when finished</t>
+  </si>
+  <si>
+    <t>Do you want to skip the final coffee ?</t>
+  </si>
+  <si>
+    <t>Brewer Cleaning Done. Press CLOSE to finish</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_COFFEE_DELIVER</t>
+  </si>
+  <si>
+    <t>Coffee delivery, please wait</t>
   </si>
 </sst>
 </file>
@@ -5761,8 +5929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12227,10 +12395,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12503,189 +12671,413 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>1712</v>
+        <v>1761</v>
       </c>
       <c r="B14" t="s">
         <v>1711</v>
       </c>
       <c r="C14" t="s">
-        <v>1745</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>1714</v>
+        <v>1762</v>
       </c>
       <c r="B15" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C15" t="s">
-        <v>1746</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>1719</v>
+        <v>1763</v>
       </c>
       <c r="B16" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="C16" t="s">
-        <v>1747</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>1720</v>
+        <v>1764</v>
       </c>
       <c r="B17" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="C17" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>1721</v>
+        <v>1765</v>
       </c>
       <c r="B18" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="C18" t="s">
-        <v>1749</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>1722</v>
+        <v>1766</v>
       </c>
       <c r="B19" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="C19" t="s">
-        <v>1750</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>1724</v>
+        <v>1767</v>
       </c>
       <c r="B20" t="s">
-        <v>1723</v>
+        <v>1717</v>
       </c>
       <c r="C20" t="s">
-        <v>1751</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>1726</v>
+        <v>1768</v>
       </c>
       <c r="B21" t="s">
-        <v>1725</v>
+        <v>1718</v>
       </c>
       <c r="C21" t="s">
-        <v>1752</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>1730</v>
+        <v>1769</v>
       </c>
       <c r="B22" t="s">
-        <v>1727</v>
+        <v>1719</v>
       </c>
       <c r="C22" t="s">
-        <v>1753</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>1731</v>
+        <v>1770</v>
       </c>
       <c r="B23" t="s">
-        <v>1728</v>
+        <v>1720</v>
       </c>
       <c r="C23" t="s">
-        <v>1754</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>1732</v>
+        <v>1771</v>
       </c>
       <c r="B24" t="s">
-        <v>1729</v>
+        <v>1721</v>
       </c>
       <c r="C24" t="s">
-        <v>1755</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>1734</v>
+        <v>1723</v>
       </c>
       <c r="B26" t="s">
-        <v>1733</v>
+        <v>1722</v>
       </c>
       <c r="C26" t="s">
-        <v>1756</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>1739</v>
+        <v>1728</v>
       </c>
       <c r="B27" t="s">
-        <v>1738</v>
+        <v>1727</v>
       </c>
       <c r="C27" t="s">
-        <v>1757</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>1740</v>
+        <v>1729</v>
       </c>
       <c r="B28" t="s">
-        <v>1735</v>
+        <v>1724</v>
       </c>
       <c r="C28" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>1741</v>
+        <v>1730</v>
       </c>
       <c r="B29" t="s">
-        <v>1744</v>
+        <v>1733</v>
       </c>
       <c r="C29" t="s">
-        <v>1759</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>1742</v>
+        <v>1731</v>
       </c>
       <c r="B30" t="s">
-        <v>1737</v>
+        <v>1726</v>
       </c>
       <c r="C30" t="s">
-        <v>1757</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>1743</v>
+        <v>1732</v>
       </c>
       <c r="B31" t="s">
-        <v>1736</v>
+        <v>1725</v>
       </c>
       <c r="C31" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B43" t="s">
         <v>1760</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Piccoli aggiustamente ai msg lavaggio sanitario vflex
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -5460,21 +5460,6 @@
     <t>$LAB_CLEANSAN_VFLEX_SKIP_COFFEE</t>
   </si>
   <si>
-    <t>LAB_CLEANSAN_VFLEX_20</t>
-  </si>
-  <si>
-    <t>LAB_CLEANSAN_VFLEX_21</t>
-  </si>
-  <si>
-    <t>LAB_CLEANSAN_VFLEX_22</t>
-  </si>
-  <si>
-    <t>LAB_CLEANSAN_VFLEX_23</t>
-  </si>
-  <si>
-    <t>LAB_CLEANSAN_VFLEX_24</t>
-  </si>
-  <si>
     <t xml:space="preserve">Brewer Rinsing </t>
   </si>
   <si>
@@ -5503,6 +5488,21 @@
   </si>
   <si>
     <t>Coffee delivery, please wait</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_20</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_21</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_22</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_23</t>
+  </si>
+  <si>
+    <t>$LAB_CLEANSAN_VFLEX_24</t>
   </si>
 </sst>
 </file>
@@ -12395,10 +12395,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12949,7 +12949,7 @@
         <v>1782</v>
       </c>
       <c r="B44" t="s">
-        <v>1811</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -12957,7 +12957,7 @@
         <v>1783</v>
       </c>
       <c r="B45" t="s">
-        <v>1812</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -13029,58 +13029,62 @@
         <v>1801</v>
       </c>
       <c r="B54" t="s">
-        <v>1813</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>1815</v>
+        <v>1810</v>
       </c>
       <c r="B55" t="s">
-        <v>1816</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B56" t="s">
         <v>1802</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1807</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B57" t="s">
         <v>1803</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1808</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B58" t="s">
         <v>1804</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1809</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B59" t="s">
         <v>1805</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>1806</v>
+        <v>1816</v>
       </c>
       <c r="B60" t="s">
-        <v>1814</v>
-      </c>
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifiche a menu prog > milker
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="1891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1895">
   <si>
     <t>LABEL</t>
   </si>
@@ -5725,6 +5725,18 @@
   </si>
   <si>
     <t>La procedura di pulizia è terminata.&lt;br&gt;&lt;br&gt;Si prega di:&lt;ul&gt;&lt;li&gt;svuotare la vaschetta dell'acqua&lt;/li&gt;&lt;li&gt;riportare il tubo del latte nella posizione iniziale&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;Premere CHIUDI per chiudere questa finestra</t>
+  </si>
+  <si>
+    <t>ENABLE CONDUCIBILITY SENSOR</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_ENABLE_CONDUCIBILITY_SENSOR</t>
+  </si>
+  <si>
+    <t>HIDRODYNAMIC EMPTYING PERIOD</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_HIDR_EMPTYING_PERIOD</t>
   </si>
 </sst>
 </file>
@@ -11474,10 +11486,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12021,6 +12033,22 @@
       </c>
       <c r="C39" s="5" t="s">
         <v>1886</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="5" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="5" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>1891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1571 primi lavori, rimane da fare l test in macchina
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="5"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1899">
   <si>
     <t>LABEL</t>
   </si>
@@ -5737,6 +5737,18 @@
   </si>
   <si>
     <t>$LAB_MILKER2_HIDR_EMPTYING_PERIOD</t>
+  </si>
+  <si>
+    <t>$LAB_CLEAN_START_GRINDER_CLEANING</t>
+  </si>
+  <si>
+    <t>START CLEANING GRINDER</t>
+  </si>
+  <si>
+    <t>$LAB_PAGE_GRINDER_CLEANING_TITLE</t>
+  </si>
+  <si>
+    <t>GRINDER CLEANING</t>
   </si>
 </sst>
 </file>
@@ -11488,7 +11500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -12920,10 +12932,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13608,6 +13620,22 @@
     <row r="61" spans="1:2">
       <c r="A61" s="2"/>
     </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1898</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizzati i messaggi per la procedura di pulizia macina #1571 e aggiunte le label per le traduzioni. Aggiunte le lingue RUSSO e TEDESCO nel menu di programmazione (file xls inviato alle relativi filiali per le traduzioni)
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="1956">
   <si>
     <t>LABEL</t>
   </si>
@@ -5739,23 +5739,194 @@
     <t>$LAB_MILKER2_HIDR_EMPTYING_PERIOD</t>
   </si>
   <si>
-    <t>$LAB_CLEAN_START_GRINDER_CLEANING</t>
-  </si>
-  <si>
-    <t>START CLEANING GRINDER</t>
-  </si>
-  <si>
-    <t>$LAB_PAGE_GRINDER_CLEANING_TITLE</t>
-  </si>
-  <si>
     <t>GRINDER CLEANING</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>НАЗАД</t>
+  </si>
+  <si>
+    <t>СПАСТИ</t>
+  </si>
+  <si>
+    <t>КНОПКА</t>
+  </si>
+  <si>
+    <t>ЗАКРЫТЬ</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>ZURÜCK</t>
+  </si>
+  <si>
+    <t>SPEICHERN</t>
+  </si>
+  <si>
+    <t>TASTE</t>
+  </si>
+  <si>
+    <t>SCHLIESSEN</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_RUNNING1</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_START</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_TITLE</t>
+  </si>
+  <si>
+    <t>PULIZIA MACINA</t>
+  </si>
+  <si>
+    <t>Running grinder cycle {0} of {1}</t>
+  </si>
+  <si>
+    <t>Macinata {0} di  {1}</t>
+  </si>
+  <si>
+    <t>Catch the product</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_CATCH</t>
+  </si>
+  <si>
+    <t>Waiting {0} sec.</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_WAIT_SECONDS</t>
+  </si>
+  <si>
+    <t>Attendere {0} sec.</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_REMOVE_BREWER_AND_BEAN</t>
+  </si>
+  <si>
+    <t>Press CONTINUE when done</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_PRESS_CONTINUE_WHEN_DONE</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_CLOSE_BEAN</t>
+  </si>
+  <si>
+    <t>Close bean hopper shutter to avoid loss of beans</t>
+  </si>
+  <si>
+    <t>Remove brewer and bean hopper</t>
+  </si>
+  <si>
+    <t>Install grinder cleaning device</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_INSTALL_GRINDER_CLEANING_DEVICE</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;WARNING:&lt;/b&gt; as soon as you press CONTINUE, the grinder will start running</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_WARN_GRINDER_RUNNING</t>
+  </si>
+  <si>
+    <t>Refill cleaning device</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_REFILL_CLEANING_DEVICE</t>
+  </si>
+  <si>
+    <t>Do you want to repeat the grinding cycles?</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_WANT_TO_REPEAT_GRINDER_CYCLE</t>
+  </si>
+  <si>
+    <t>Put back  bean hopper</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_PUT_BACK_BEAN_HOPPER</t>
+  </si>
+  <si>
+    <t>Open hopper shutter</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_OPEN_HOPPER_SHUTTER</t>
+  </si>
+  <si>
+    <t>Put brewer back into position</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_PUT_BREWER_INTO_POSITION</t>
+  </si>
+  <si>
+    <t>Do you want do dispense a coffe?</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_WANT_COFFEE</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;ATTENZIONE&lt;/b&gt;. Non appena premuto CONTINUA, la macina inizierà a macinare</t>
+  </si>
+  <si>
+    <t>Riempire il dispositivo di pulizia</t>
+  </si>
+  <si>
+    <t>Rimuovere il gruppo infusione ed il contenitore caffè in grani</t>
+  </si>
+  <si>
+    <t>Usare un bicchiere per recuperare il prodotto macinato</t>
+  </si>
+  <si>
+    <t>Installare il dispositivo di pulizia della macina</t>
+  </si>
+  <si>
+    <t>Premere CONTINUA quando fatto</t>
+  </si>
+  <si>
+    <t>Si vuole ripetere l'operazione di macinatura?</t>
+  </si>
+  <si>
+    <t>Rimettere il contenitore caffè in posizione</t>
+  </si>
+  <si>
+    <t>Aprire la saracinesca del contenitore caffè in grani</t>
+  </si>
+  <si>
+    <t>Chiudere la saracinesca del contenitore caffè per evitare di perdere grani</t>
+  </si>
+  <si>
+    <t>Please select which grinder you'd like to clean, then press CONTINUE to continue or ABORT to terminate</t>
+  </si>
+  <si>
+    <t>$LAB_GRINDERCLEANING_PLEASE_SELECT_GRINDER</t>
+  </si>
+  <si>
+    <t>Prego selezionare la macina che si desidera pulire. Premere CONTINUA per proseguire, ABORT per terminare</t>
+  </si>
+  <si>
+    <t>START CLEANING&lt;br&gt;GRINDER</t>
+  </si>
+  <si>
+    <t>PULIZIA&lt;br&gt;MACINA</t>
+  </si>
+  <si>
+    <t>Rimettere il gruppo infusione in posizione</t>
+  </si>
+  <si>
+    <t>Si vuole erogare un caffè?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5804,6 +5975,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5831,7 +6009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5890,6 +6068,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -6170,10 +6349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6184,10 +6363,11 @@
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6209,8 +6389,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
@@ -6232,8 +6418,14 @@
       <c r="G2" s="10" t="s">
         <v>1441</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
+      <c r="H2" t="s">
+        <v>1897</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -6255,8 +6447,14 @@
       <c r="G3" s="10" t="s">
         <v>1442</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75">
+      <c r="H3" t="s">
+        <v>1898</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>546</v>
       </c>
@@ -6273,7 +6471,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>377</v>
       </c>
@@ -6296,7 +6494,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" t="s">
         <v>158</v>
       </c>
@@ -6319,7 +6517,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -6342,7 +6540,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>962</v>
       </c>
@@ -6356,7 +6554,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" t="s">
         <v>531</v>
       </c>
@@ -6378,8 +6576,14 @@
       <c r="G9" s="10" t="s">
         <v>1447</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75">
+      <c r="H9" t="s">
+        <v>1899</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" t="s">
         <v>907</v>
       </c>
@@ -6401,8 +6605,14 @@
       <c r="G10" s="10" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75">
+      <c r="H10" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -6425,7 +6635,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>135</v>
       </c>
@@ -6448,7 +6658,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75">
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>522</v>
       </c>
@@ -6471,7 +6681,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1431</v>
       </c>
@@ -6482,7 +6692,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>1420</v>
       </c>
@@ -6493,7 +6703,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75">
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -7208,7 +7418,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.75">
+    <row r="49" spans="1:7" ht="31.5">
       <c r="A49" s="3" t="s">
         <v>587</v>
       </c>
@@ -7647,11 +7857,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7661,10 +7869,11 @@
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7686,8 +7895,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -7707,7 +7922,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -7727,7 +7942,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -7747,7 +7962,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -7770,7 +7985,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -7793,7 +8008,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -7816,7 +8031,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -7836,7 +8051,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -7859,7 +8074,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -7882,7 +8097,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -7902,7 +8117,7 @@
         <v>1609</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -7925,7 +8140,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -7948,7 +8163,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -7971,7 +8186,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>725</v>
       </c>
@@ -7994,7 +8209,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>724</v>
       </c>
@@ -8109,7 +8324,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="45">
       <c r="A21" t="s">
         <v>245</v>
       </c>
@@ -8132,7 +8347,7 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="45">
       <c r="A22" t="s">
         <v>248</v>
       </c>
@@ -8155,7 +8370,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="45">
       <c r="A23" t="s">
         <v>247</v>
       </c>
@@ -8213,7 +8428,7 @@
         <v>1621</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="45">
       <c r="A26" t="s">
         <v>250</v>
       </c>
@@ -8236,7 +8451,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" t="s">
         <v>253</v>
       </c>
@@ -8419,11 +8634,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8433,10 +8646,11 @@
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8458,8 +8672,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>263</v>
       </c>
@@ -8482,7 +8702,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" t="s">
         <v>270</v>
       </c>
@@ -8505,7 +8725,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>268</v>
       </c>
@@ -8528,7 +8748,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" t="s">
         <v>287</v>
       </c>
@@ -8548,7 +8768,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -8571,7 +8791,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" t="s">
         <v>273</v>
       </c>
@@ -8594,7 +8814,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -8617,7 +8837,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -8640,7 +8860,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>282</v>
       </c>
@@ -8663,7 +8883,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -8686,7 +8906,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" t="s">
         <v>290</v>
       </c>
@@ -8709,7 +8929,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -8732,7 +8952,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" t="s">
         <v>297</v>
       </c>
@@ -8755,7 +8975,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9" ht="30">
       <c r="A15" t="s">
         <v>300</v>
       </c>
@@ -8778,7 +8998,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:9" ht="75">
       <c r="A16" t="s">
         <v>303</v>
       </c>
@@ -8847,7 +9067,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="3" t="s">
         <v>695</v>
       </c>
@@ -8881,7 +9101,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" t="s">
         <v>898</v>
       </c>
@@ -8924,7 +9144,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="60">
       <c r="A23" t="s">
         <v>903</v>
       </c>
@@ -9032,11 +9252,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9046,9 +9264,10 @@
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9070,8 +9289,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>309</v>
       </c>
@@ -9094,7 +9319,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>316</v>
       </c>
@@ -9117,7 +9342,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>315</v>
       </c>
@@ -9140,7 +9365,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -9163,7 +9388,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>590</v>
       </c>
@@ -9193,11 +9418,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9208,9 +9431,10 @@
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9232,8 +9456,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -9256,7 +9486,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -9279,7 +9509,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>331</v>
       </c>
@@ -9302,7 +9532,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>334</v>
       </c>
@@ -9332,11 +9562,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9346,10 +9574,11 @@
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -9371,8 +9600,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>340</v>
       </c>
@@ -9393,7 +9628,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>344</v>
       </c>
@@ -9414,7 +9649,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>348</v>
       </c>
@@ -9437,7 +9672,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>349</v>
       </c>
@@ -9460,7 +9695,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>350</v>
       </c>
@@ -9477,7 +9712,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9" ht="45">
       <c r="A7" s="5" t="s">
         <v>354</v>
       </c>
@@ -9500,7 +9735,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>358</v>
       </c>
@@ -9521,7 +9756,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
         <v>360</v>
       </c>
@@ -9544,7 +9779,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>361</v>
       </c>
@@ -9567,7 +9802,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>366</v>
       </c>
@@ -9588,7 +9823,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>369</v>
       </c>
@@ -9611,7 +9846,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="5" t="s">
         <v>373</v>
       </c>
@@ -9632,7 +9867,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>375</v>
       </c>
@@ -9655,7 +9890,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
         <v>382</v>
       </c>
@@ -9678,7 +9913,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
         <v>387</v>
       </c>
@@ -9777,11 +10012,9 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9789,12 +10022,12 @@
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9816,8 +10049,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -9840,7 +10079,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>227</v>
       </c>
@@ -9863,7 +10102,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -9886,7 +10125,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>237</v>
       </c>
@@ -9909,7 +10148,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" t="s">
         <v>236</v>
       </c>
@@ -9929,7 +10168,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -9959,11 +10198,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9973,11 +10210,12 @@
     <col min="4" max="4" width="9.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="7" style="5" customWidth="1"/>
-    <col min="7" max="7" width="90" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="7" width="25.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="62.42578125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1">
+    <row r="1" spans="1:9" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -9999,8 +10237,14 @@
       <c r="G1" s="7" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>535</v>
       </c>
@@ -10023,7 +10267,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33" customHeight="1">
+    <row r="3" spans="1:9" ht="33" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>536</v>
       </c>
@@ -10046,7 +10290,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24" customHeight="1">
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>538</v>
       </c>
@@ -10069,7 +10313,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.5" customHeight="1">
+    <row r="5" spans="1:9" ht="22.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>541</v>
       </c>
@@ -10092,7 +10336,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="23.25" customHeight="1">
+    <row r="6" spans="1:9" ht="23.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>544</v>
       </c>
@@ -10115,7 +10359,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25.5" customHeight="1">
+    <row r="7" spans="1:9" ht="25.5" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>548</v>
       </c>
@@ -10138,7 +10382,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.25" customHeight="1">
+    <row r="8" spans="1:9" ht="26.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>553</v>
       </c>
@@ -10161,11 +10405,11 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="F9" s="6"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" ht="27.75" customHeight="1">
+    <row r="10" spans="1:9" ht="27.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>556</v>
       </c>
@@ -10188,7 +10432,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="23.25" customHeight="1">
+    <row r="11" spans="1:9" ht="23.25" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>558</v>
       </c>
@@ -10211,11 +10455,11 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="F12" s="6"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="21.75" customHeight="1">
+    <row r="13" spans="1:9" ht="21.75" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>565</v>
       </c>
@@ -10238,11 +10482,11 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75">
+    <row r="14" spans="1:9" ht="15.75">
       <c r="F14" s="6"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="29.25" customHeight="1">
+    <row r="15" spans="1:9" ht="29.25" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>567</v>
       </c>
@@ -10265,7 +10509,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="26.25" customHeight="1">
+    <row r="16" spans="1:9" ht="26.25" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>569</v>
       </c>
@@ -10488,11 +10732,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10500,10 +10742,11 @@
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="4" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10525,8 +10768,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>680</v>
       </c>
@@ -10549,7 +10798,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>681</v>
       </c>
@@ -10572,7 +10821,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>682</v>
       </c>
@@ -10586,7 +10835,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>683</v>
       </c>
@@ -10609,7 +10858,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>704</v>
       </c>
@@ -10632,7 +10881,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>707</v>
       </c>
@@ -10655,7 +10904,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>684</v>
       </c>
@@ -10678,7 +10927,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>685</v>
       </c>
@@ -10701,7 +10950,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>686</v>
       </c>
@@ -10724,7 +10973,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="21" customHeight="1">
+    <row r="11" spans="1:9" ht="21" customHeight="1">
       <c r="A11" t="s">
         <v>687</v>
       </c>
@@ -10747,7 +10996,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>688</v>
       </c>
@@ -10770,7 +11019,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>689</v>
       </c>
@@ -10793,7 +11042,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>690</v>
       </c>
@@ -10816,7 +11065,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>691</v>
       </c>
@@ -10839,7 +11088,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>692</v>
       </c>
@@ -10873,11 +11122,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.7109375" defaultRowHeight="15"/>
   <cols>
@@ -10886,10 +11133,11 @@
     <col min="4" max="4" width="12.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="36.7109375" style="5"/>
+    <col min="7" max="7" width="16" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="36.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -10911,8 +11159,14 @@
       <c r="G1" s="7" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>858</v>
       </c>
@@ -10935,7 +11189,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>861</v>
       </c>
@@ -10958,7 +11212,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>865</v>
       </c>
@@ -10981,7 +11235,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>866</v>
       </c>
@@ -11004,7 +11258,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30.75" customHeight="1">
+    <row r="6" spans="1:9" ht="30.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>871</v>
       </c>
@@ -11027,7 +11281,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>873</v>
       </c>
@@ -11050,7 +11304,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>875</v>
       </c>
@@ -11073,10 +11327,10 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:9" ht="31.5">
       <c r="A10" s="5" t="s">
         <v>886</v>
       </c>
@@ -11099,7 +11353,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.5">
+    <row r="11" spans="1:9" ht="63">
       <c r="A11" s="5" t="s">
         <v>890</v>
       </c>
@@ -11122,7 +11376,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
+    <row r="12" spans="1:9" ht="31.5">
       <c r="A12" s="5" t="s">
         <v>916</v>
       </c>
@@ -11145,7 +11399,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75">
+    <row r="13" spans="1:9" ht="31.5">
       <c r="A13" s="5" t="s">
         <v>917</v>
       </c>
@@ -11168,7 +11422,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="47.25">
+    <row r="14" spans="1:9" ht="126">
       <c r="A14" s="5" t="s">
         <v>918</v>
       </c>
@@ -11198,11 +11452,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -11211,10 +11463,11 @@
     <col min="3" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -11236,8 +11489,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>200</v>
       </c>
@@ -11260,7 +11519,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>201</v>
       </c>
@@ -11283,7 +11542,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9" ht="75">
       <c r="A4" s="5" t="s">
         <v>202</v>
       </c>
@@ -11306,7 +11565,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="5" t="s">
         <v>203</v>
       </c>
@@ -11329,7 +11588,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="5" t="s">
         <v>204</v>
       </c>
@@ -11352,7 +11611,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="5" t="s">
         <v>205</v>
       </c>
@@ -11375,7 +11634,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>206</v>
       </c>
@@ -11398,7 +11657,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="5" t="s">
         <v>207</v>
       </c>
@@ -11421,7 +11680,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>208</v>
       </c>
@@ -11444,7 +11703,7 @@
         <v>1551</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>210</v>
       </c>
@@ -11467,7 +11726,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>209</v>
       </c>
@@ -11498,25 +11757,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="79.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19" style="5" customWidth="1"/>
     <col min="4" max="4" width="6" style="5" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="5"/>
     <col min="6" max="6" width="6.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="7" width="11.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="49.5703125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1">
+    <row r="1" spans="1:9" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -11538,8 +11796,14 @@
       <c r="G1" s="7" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>504</v>
       </c>
@@ -11562,7 +11826,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>506</v>
       </c>
@@ -11585,7 +11849,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>508</v>
       </c>
@@ -11608,7 +11872,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>510</v>
       </c>
@@ -11631,7 +11895,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="5" t="s">
         <v>513</v>
       </c>
@@ -11654,7 +11918,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9" ht="60">
       <c r="A7" s="5" t="s">
         <v>514</v>
       </c>
@@ -11674,7 +11938,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="5" t="s">
         <v>516</v>
       </c>
@@ -11697,7 +11961,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9" ht="45">
       <c r="A9" s="5" t="s">
         <v>518</v>
       </c>
@@ -11720,7 +11984,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" s="5" t="s">
         <v>702</v>
       </c>
@@ -11743,7 +12007,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>1423</v>
       </c>
@@ -11754,7 +12018,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>1426</v>
       </c>
@@ -11765,7 +12029,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="8" t="s">
         <v>1428</v>
       </c>
@@ -11773,7 +12037,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>1430</v>
       </c>
@@ -11781,7 +12045,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
         <v>1810</v>
       </c>
@@ -11792,7 +12056,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
         <v>1826</v>
       </c>
@@ -12073,9 +12337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12083,10 +12345,11 @@
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -12108,8 +12371,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>395</v>
       </c>
@@ -12132,7 +12401,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>400</v>
       </c>
@@ -12155,7 +12424,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>402</v>
       </c>
@@ -12178,7 +12447,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>406</v>
       </c>
@@ -12201,7 +12470,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>409</v>
       </c>
@@ -12224,7 +12493,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>412</v>
       </c>
@@ -12247,7 +12516,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="5" t="s">
         <v>414</v>
       </c>
@@ -12268,7 +12537,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="5" t="s">
         <v>417</v>
       </c>
@@ -12289,7 +12558,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>421</v>
       </c>
@@ -12310,7 +12579,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9" ht="45">
       <c r="A11" s="5" t="s">
         <v>423</v>
       </c>
@@ -12333,7 +12602,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="5" t="s">
         <v>426</v>
       </c>
@@ -12356,7 +12625,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="5" t="s">
         <v>428</v>
       </c>
@@ -12377,7 +12646,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>431</v>
       </c>
@@ -12400,7 +12669,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9" ht="30">
       <c r="A15" s="5" t="s">
         <v>433</v>
       </c>
@@ -12423,7 +12692,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
         <v>436</v>
       </c>
@@ -12469,7 +12738,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="60">
       <c r="A18" s="5" t="s">
         <v>442</v>
       </c>
@@ -12515,7 +12784,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="30">
       <c r="A20" s="5" t="s">
         <v>451</v>
       </c>
@@ -12656,11 +12925,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12669,10 +12936,11 @@
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12694,8 +12962,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>453</v>
       </c>
@@ -12718,7 +12992,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>454</v>
       </c>
@@ -12741,7 +13015,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>458</v>
       </c>
@@ -12764,7 +13038,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>461</v>
       </c>
@@ -12787,7 +13061,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>463</v>
       </c>
@@ -12810,7 +13084,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>464</v>
       </c>
@@ -12833,7 +13107,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>469</v>
       </c>
@@ -12856,7 +13130,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>472</v>
       </c>
@@ -12879,7 +13153,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>475</v>
       </c>
@@ -12902,7 +13176,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>477</v>
       </c>
@@ -12932,23 +13206,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12970,8 +13243,14 @@
       <c r="G1" s="1" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -12994,7 +13273,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -13017,7 +13296,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -13040,7 +13319,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -13063,7 +13342,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -13086,7 +13365,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -13109,7 +13388,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -13132,7 +13411,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -13155,7 +13434,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -13178,7 +13457,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>955</v>
       </c>
@@ -13192,7 +13471,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>957</v>
       </c>
@@ -13206,7 +13485,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1753</v>
       </c>
@@ -13217,7 +13496,7 @@
         <v>1726</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>1754</v>
       </c>
@@ -13228,7 +13507,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>1755</v>
       </c>
@@ -13521,7 +13800,7 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>1787</v>
       </c>
@@ -13529,7 +13808,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>1788</v>
       </c>
@@ -13537,7 +13816,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>1789</v>
       </c>
@@ -13545,7 +13824,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>1790</v>
       </c>
@@ -13553,7 +13832,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>1791</v>
       </c>
@@ -13561,7 +13840,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>1793</v>
       </c>
@@ -13569,7 +13848,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>1802</v>
       </c>
@@ -13577,7 +13856,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>1804</v>
       </c>
@@ -13585,7 +13864,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>1805</v>
       </c>
@@ -13593,7 +13872,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>1806</v>
       </c>
@@ -13601,7 +13880,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>1807</v>
       </c>
@@ -13609,7 +13888,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>1808</v>
       </c>
@@ -13617,23 +13896,194 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B62" t="s">
         <v>1895</v>
       </c>
-      <c r="B62" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>1897</v>
+        <v>1907</v>
       </c>
       <c r="B63" t="s">
-        <v>1898</v>
+        <v>1952</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1914</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1925</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
piccola correzione nel messaggio finale "do you want a coffeE" del lavaggio grinder, mancava una E in coffee
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -5865,9 +5865,6 @@
     <t>$LAB_GRINDERCLEANING_PUT_BREWER_INTO_POSITION</t>
   </si>
   <si>
-    <t>Do you want do dispense a coffe?</t>
-  </si>
-  <si>
     <t>$LAB_GRINDERCLEANING_WANT_COFFEE</t>
   </si>
   <si>
@@ -5920,6 +5917,9 @@
   </si>
   <si>
     <t>Si vuole erogare un caffè?</t>
+  </si>
+  <si>
+    <t>Do you want do dispense a coffee?</t>
   </si>
 </sst>
 </file>
@@ -6351,7 +6351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -13208,7 +13208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13915,21 +13917,21 @@
         <v>1907</v>
       </c>
       <c r="B63" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C63" t="s">
         <v>1952</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1953</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C64" t="s">
         <v>1950</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1949</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1951</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -13951,7 +13953,7 @@
         <v>1912</v>
       </c>
       <c r="C66" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -13973,7 +13975,7 @@
         <v>1921</v>
       </c>
       <c r="C68" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -13984,7 +13986,7 @@
         <v>1922</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -13995,7 +13997,7 @@
         <v>1923</v>
       </c>
       <c r="C70" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -14006,7 +14008,7 @@
         <v>1918</v>
       </c>
       <c r="C71" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -14017,7 +14019,7 @@
         <v>1925</v>
       </c>
       <c r="C72" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -14028,7 +14030,7 @@
         <v>1927</v>
       </c>
       <c r="C73" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -14039,7 +14041,7 @@
         <v>1929</v>
       </c>
       <c r="C74" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -14050,7 +14052,7 @@
         <v>1931</v>
       </c>
       <c r="C75" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -14061,7 +14063,7 @@
         <v>1933</v>
       </c>
       <c r="C76" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -14072,18 +14074,18 @@
         <v>1935</v>
       </c>
       <c r="C77" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B78" t="s">
-        <v>1937</v>
+        <v>1955</v>
       </c>
       <c r="C78" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rheamedia Nestle2.5, punti 11.17.18.21.22.24.27.28.30.39.42.44.45
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="1979">
   <si>
     <t>LABEL</t>
   </si>
@@ -5962,6 +5962,33 @@
   </si>
   <si>
     <t>Nada para mostrar</t>
+  </si>
+  <si>
+    <t>PROG MENU PIN CODE</t>
+  </si>
+  <si>
+    <t>QUICK MENU PIN CODE</t>
+  </si>
+  <si>
+    <t>$LAB_PROG_MENU_PIN_CODE</t>
+  </si>
+  <si>
+    <t>$LAB_QUICK_MENU_PIN_CODE</t>
+  </si>
+  <si>
+    <t>ARE YOU SURE YOU WISH TO LAUNCH THE CHOSEN OPERATION?</t>
+  </si>
+  <si>
+    <t>$LAB_ARE_YOU_SURE_YOU_WISH_TO_LAUNCH</t>
+  </si>
+  <si>
+    <t>SEI SICURO DI VOLERE AVVIARE L'OPERAZIONE SCELTA?</t>
+  </si>
+  <si>
+    <t>ÊTES-VOUS SR DE SOUHAITER LANCER L'OPÉRATION CHOISIE ?</t>
+  </si>
+  <si>
+    <t>¿Estás seguro de que deseas lanzar la operación elegida?</t>
   </si>
 </sst>
 </file>
@@ -6394,10 +6421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7889,6 +7916,23 @@
       </c>
       <c r="G67" s="10" t="s">
         <v>1496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="3" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>1978</v>
       </c>
     </row>
   </sheetData>
@@ -12434,9 +12478,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13015,6 +13061,22 @@
       <c r="F27" s="5"/>
       <c r="J27" t="s">
         <v>941</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="5" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="5" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementazione descaling lato GPU TS, passo a linux per il build
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="1979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="2023">
   <si>
     <t>LABEL</t>
   </si>
@@ -5989,6 +5989,138 @@
   </si>
   <si>
     <t>¿Estás seguro de que deseas lanzar la operación elegida?</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_START</t>
+  </si>
+  <si>
+    <t>START DESCALING</t>
+  </si>
+  <si>
+    <t>DECALCIFICAZIONE</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_PRESS_CONTINUE</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_OPEN_BOILER_TAP</t>
+  </si>
+  <si>
+    <t>Open boiler tap</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_CLOSE_BOILER_TAP</t>
+  </si>
+  <si>
+    <t>Close boiler tap</t>
+  </si>
+  <si>
+    <t>please wait...</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_PLS_WAIT</t>
+  </si>
+  <si>
+    <t>Emptying hydraulic circuit</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_2</t>
+  </si>
+  <si>
+    <t>Attach submersible pump to the tank containing descaling detergent</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_4</t>
+  </si>
+  <si>
+    <t>Filling hydraulic circuit with descaling detergent</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_5</t>
+  </si>
+  <si>
+    <t>Check descaling detergent level in the air tank</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_6</t>
+  </si>
+  <si>
+    <t>Starting to fill hydraulic tubes with descaling detergent</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_7</t>
+  </si>
+  <si>
+    <t>Please wait for the descaling liquid action...</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_8</t>
+  </si>
+  <si>
+    <t>Descaling liquid starts draining through the nozzles</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_9</t>
+  </si>
+  <si>
+    <t>Check the liquid colour drained from the nozzles, it defines if descaling process successfully completed.&lt;br&gt;Press CONTINUE button to continue, or press REPEAT to repeat previous steps.</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_10</t>
+  </si>
+  <si>
+    <t>Emptying hydraulic circuit. All descaling liquid drain out through the nozzles</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_12</t>
+  </si>
+  <si>
+    <t>Change supply source to water tank. Attach submersible pump to the tank containing water</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_14</t>
+  </si>
+  <si>
+    <t>Hydraulic circuit will be filled with water</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_15</t>
+  </si>
+  <si>
+    <t>Check water level into the air tank</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_16</t>
+  </si>
+  <si>
+    <t>Water drained out through nozzles</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_17</t>
+  </si>
+  <si>
+    <t>Dispense water and test the sample. Place a cup to collect the sample</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_18</t>
+  </si>
+  <si>
+    <t>Start draining sample through each nozzle</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_19</t>
+  </si>
+  <si>
+    <t>Check the pH of collected sample. Press CONTINUE button to continue or REPEAT to repeat the previous steps to clean properly the hydraulic circuit.</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_20</t>
+  </si>
+  <si>
+    <t>Descaling procedure finished</t>
+  </si>
+  <si>
+    <t>$LAB_DESCALING_21</t>
   </si>
 </sst>
 </file>
@@ -6423,8 +6555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13367,10 +13499,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14249,6 +14381,185 @@
         <v>1954</v>
       </c>
     </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Alcune correzioni ai msg per il descaling Modifiche all'inserimento dei PIN code, il tasto "0" non deve esistere
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801" activeTab="8"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="24765" windowHeight="11775" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="2023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="2026">
   <si>
     <t>LABEL</t>
   </si>
@@ -6069,9 +6069,6 @@
     <t>$LAB_DESCALING_10</t>
   </si>
   <si>
-    <t>Emptying hydraulic circuit. All descaling liquid drain out through the nozzles</t>
-  </si>
-  <si>
     <t>$LAB_DESCALING_12</t>
   </si>
   <si>
@@ -6117,10 +6114,22 @@
     <t>$LAB_DESCALING_20</t>
   </si>
   <si>
-    <t>Descaling procedure finished</t>
-  </si>
-  <si>
     <t>$LAB_DESCALING_21</t>
+  </si>
+  <si>
+    <t>Descaling procedure finished,  press CLOSE to finish</t>
+  </si>
+  <si>
+    <t>$LAB_SET_PIN</t>
+  </si>
+  <si>
+    <t>SET PIN</t>
+  </si>
+  <si>
+    <t>$LAB_RESET_PIN</t>
+  </si>
+  <si>
+    <t>RESET PIN</t>
   </si>
 </sst>
 </file>
@@ -6553,10 +6562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8065,6 +8074,22 @@
       </c>
       <c r="E68" s="3" t="s">
         <v>1978</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="3" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="3" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>
@@ -13501,8 +13526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14490,71 +14515,71 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B93" t="s">
-        <v>2005</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B94" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B95" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B96" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B97" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B98" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B99" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B100" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="B101" t="s">
         <v>2021</v>

</xml_diff>

<commit_message>
Aggiunta colonna "M" nel file excel delle traduzioni in modo da supportare il JP
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="8"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4492" uniqueCount="3946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4507" uniqueCount="3947">
   <si>
     <t>LABEL</t>
   </si>
@@ -11887,6 +11887,9 @@
   </si>
   <si>
     <t>Check the collected sample. Press CONTINUE button to continue or REPEAT to repeat the previous steps to clean properly the hydraulic circuit.</t>
+  </si>
+  <si>
+    <t>JP</t>
   </si>
 </sst>
 </file>
@@ -12393,10 +12396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12411,7 +12414,7 @@
     <col min="8" max="8" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12448,8 +12451,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
@@ -12487,7 +12493,7 @@
         <v>3258</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -12525,7 +12531,7 @@
         <v>3259</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:13" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>544</v>
       </c>
@@ -12560,7 +12566,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>375</v>
       </c>
@@ -12598,7 +12604,7 @@
         <v>3261</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:13" ht="15.75">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -12636,7 +12642,7 @@
         <v>3262</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -12674,7 +12680,7 @@
         <v>3263</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>903</v>
       </c>
@@ -12707,7 +12713,7 @@
         <v>3264</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" t="s">
         <v>529</v>
       </c>
@@ -12745,7 +12751,7 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:13" ht="15.75">
       <c r="A10" t="s">
         <v>852</v>
       </c>
@@ -12783,7 +12789,7 @@
         <v>3266</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:13" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -12821,7 +12827,7 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:13" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>133</v>
       </c>
@@ -12859,7 +12865,7 @@
         <v>3266</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:13" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>520</v>
       </c>
@@ -12897,7 +12903,7 @@
         <v>3268</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>1323</v>
       </c>
@@ -12930,7 +12936,7 @@
         <v>3269</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>1312</v>
       </c>
@@ -12963,7 +12969,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:13" ht="15.75">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -14960,25 +14966,25 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15015,8 +15021,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -15054,7 +15063,7 @@
         <v>3523</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -15092,7 +15101,7 @@
         <v>3524</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -15130,7 +15139,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -15168,7 +15177,7 @@
         <v>3526</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -15206,7 +15215,7 @@
         <v>3527</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -15244,7 +15253,7 @@
         <v>3528</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -15282,7 +15291,7 @@
         <v>3529</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -15320,7 +15329,7 @@
         <v>3530</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -15358,7 +15367,7 @@
         <v>3531</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -15396,7 +15405,7 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -15434,7 +15443,7 @@
         <v>3533</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -15472,7 +15481,7 @@
         <v>3534</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -15510,7 +15519,7 @@
         <v>3535</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>714</v>
       </c>
@@ -15548,7 +15557,7 @@
         <v>3536</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>713</v>
       </c>
@@ -16268,28 +16277,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16326,8 +16335,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>261</v>
       </c>
@@ -16363,7 +16375,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:13" ht="30">
       <c r="A3" t="s">
         <v>268</v>
       </c>
@@ -16401,7 +16413,7 @@
         <v>3556</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:13" ht="30">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -16439,7 +16451,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -16477,7 +16489,7 @@
         <v>3558</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45">
+    <row r="6" spans="1:13" ht="45">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -16513,7 +16525,7 @@
         <v>3559</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -16551,7 +16563,7 @@
         <v>3560</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>275</v>
       </c>
@@ -16589,7 +16601,7 @@
         <v>3561</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>278</v>
       </c>
@@ -16627,7 +16639,7 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>280</v>
       </c>
@@ -16665,7 +16677,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:13" ht="30">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -16703,7 +16715,7 @@
         <v>3564</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30">
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -16741,7 +16753,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" t="s">
         <v>292</v>
       </c>
@@ -16779,7 +16791,7 @@
         <v>3566</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -16817,7 +16829,7 @@
         <v>3567</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30">
+    <row r="15" spans="1:13" ht="30">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -16855,7 +16867,7 @@
         <v>3568</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="75">
+    <row r="16" spans="1:13" ht="75">
       <c r="A16" t="s">
         <v>301</v>
       </c>
@@ -17386,26 +17398,27 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="56.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17442,8 +17455,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -17481,7 +17497,7 @@
         <v>3584</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>314</v>
       </c>
@@ -17519,7 +17535,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>313</v>
       </c>
@@ -17557,7 +17573,7 @@
         <v>3586</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>316</v>
       </c>
@@ -17595,7 +17611,7 @@
         <v>3264</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>588</v>
       </c>
@@ -17640,10 +17656,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17651,17 +17667,18 @@
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1"/>
-    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17698,8 +17715,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -17737,7 +17757,7 @@
         <v>3588</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>326</v>
       </c>
@@ -17775,7 +17795,7 @@
         <v>3589</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>329</v>
       </c>
@@ -17813,7 +17833,7 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>332</v>
       </c>
@@ -17858,28 +17878,29 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -17916,8 +17937,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>338</v>
       </c>
@@ -17955,7 +17979,7 @@
         <v>3592</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>342</v>
       </c>
@@ -17993,7 +18017,7 @@
         <v>3593</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>346</v>
       </c>
@@ -18031,7 +18055,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
         <v>347</v>
       </c>
@@ -18069,7 +18093,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>348</v>
       </c>
@@ -18103,7 +18127,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45">
+    <row r="7" spans="1:13" ht="45">
       <c r="A7" s="4" t="s">
         <v>352</v>
       </c>
@@ -18141,7 +18165,7 @@
         <v>3594</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>356</v>
       </c>
@@ -18179,7 +18203,7 @@
         <v>3595</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
         <v>358</v>
       </c>
@@ -18217,7 +18241,7 @@
         <v>3596</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>359</v>
       </c>
@@ -18255,7 +18279,7 @@
         <v>3597</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
         <v>364</v>
       </c>
@@ -18293,7 +18317,7 @@
         <v>3598</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
         <v>367</v>
       </c>
@@ -18331,7 +18355,7 @@
         <v>3599</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>371</v>
       </c>
@@ -18369,7 +18393,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
         <v>373</v>
       </c>
@@ -18407,7 +18431,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
         <v>380</v>
       </c>
@@ -18445,7 +18469,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
         <v>385</v>
       </c>
@@ -18604,10 +18628,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18615,17 +18639,19 @@
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18662,8 +18688,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>223</v>
       </c>
@@ -18701,7 +18730,7 @@
         <v>3551</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>225</v>
       </c>
@@ -18739,7 +18768,7 @@
         <v>3605</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -18777,7 +18806,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>235</v>
       </c>
@@ -18815,7 +18844,7 @@
         <v>3606</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -18853,7 +18882,7 @@
         <v>3607</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" t="s">
         <v>236</v>
       </c>
@@ -18891,7 +18920,7 @@
         <v>3608</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>1840</v>
       </c>
@@ -18902,7 +18931,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>1843</v>
       </c>
@@ -18932,10 +18961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -18952,7 +18981,7 @@
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1">
+    <row r="1" spans="1:13" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -18989,8 +19018,11 @@
       <c r="L1" s="34" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M1" s="6" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>533</v>
       </c>
@@ -19028,7 +19060,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="33" customHeight="1">
+    <row r="3" spans="1:13" ht="33" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>534</v>
       </c>
@@ -19066,7 +19098,7 @@
         <v>3321</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1">
+    <row r="4" spans="1:13" ht="24" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>536</v>
       </c>
@@ -19104,7 +19136,7 @@
         <v>3322</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="22.5" customHeight="1">
+    <row r="5" spans="1:13" ht="22.5" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>539</v>
       </c>
@@ -19142,7 +19174,7 @@
         <v>3323</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="23.25" customHeight="1">
+    <row r="6" spans="1:13" ht="23.25" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>542</v>
       </c>
@@ -19180,7 +19212,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="25.5" customHeight="1">
+    <row r="7" spans="1:13" ht="25.5" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>546</v>
       </c>
@@ -19218,7 +19250,7 @@
         <v>3325</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="26.25" customHeight="1">
+    <row r="8" spans="1:13" ht="26.25" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>551</v>
       </c>
@@ -19256,7 +19288,7 @@
         <v>3326</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="B9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -19268,7 +19300,7 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
     </row>
-    <row r="10" spans="1:12" ht="27.75" customHeight="1">
+    <row r="10" spans="1:13" ht="27.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>554</v>
       </c>
@@ -19304,7 +19336,7 @@
         <v>3327</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="23.25" customHeight="1">
+    <row r="11" spans="1:13" ht="23.25" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>556</v>
       </c>
@@ -19340,7 +19372,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:13" ht="15.75">
       <c r="B12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -19352,7 +19384,7 @@
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
     </row>
-    <row r="13" spans="1:12" ht="21.75" customHeight="1">
+    <row r="13" spans="1:13" ht="21.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>563</v>
       </c>
@@ -19388,7 +19420,7 @@
         <v>3329</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:13" ht="15.75">
       <c r="B14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -19400,7 +19432,7 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="1:12" ht="29.25" customHeight="1">
+    <row r="15" spans="1:13" ht="29.25" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>565</v>
       </c>
@@ -19436,7 +19468,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="26.25" customHeight="1">
+    <row r="16" spans="1:13" ht="26.25" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>567</v>
       </c>
@@ -20037,10 +20069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H16"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20053,7 +20085,7 @@
     <col min="8" max="8" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20090,8 +20122,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>670</v>
       </c>
@@ -20129,7 +20164,7 @@
         <v>3341</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>671</v>
       </c>
@@ -20167,7 +20202,7 @@
         <v>3342</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>672</v>
       </c>
@@ -20200,7 +20235,7 @@
         <v>3343</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>673</v>
       </c>
@@ -20238,7 +20273,7 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>694</v>
       </c>
@@ -20276,7 +20311,7 @@
         <v>3344</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>697</v>
       </c>
@@ -20314,7 +20349,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>674</v>
       </c>
@@ -20352,7 +20387,7 @@
         <v>3346</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>675</v>
       </c>
@@ -20390,7 +20425,7 @@
         <v>3347</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>676</v>
       </c>
@@ -20428,7 +20463,7 @@
         <v>3348</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="21" customHeight="1">
+    <row r="11" spans="1:13" ht="21" customHeight="1">
       <c r="A11" t="s">
         <v>677</v>
       </c>
@@ -20466,7 +20501,7 @@
         <v>3349</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>678</v>
       </c>
@@ -20504,7 +20539,7 @@
         <v>3350</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>679</v>
       </c>
@@ -20542,7 +20577,7 @@
         <v>3351</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>680</v>
       </c>
@@ -20580,7 +20615,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>681</v>
       </c>
@@ -20618,7 +20653,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>682</v>
       </c>
@@ -20667,26 +20702,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="36.7109375" style="4"/>
-    <col min="3" max="3" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="16" style="4" customWidth="1"/>
-    <col min="8" max="9" width="36.7109375" style="4"/>
-    <col min="10" max="10" width="125.42578125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="36.7109375" style="4"/>
+    <col min="8" max="8" width="4.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="36.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -20723,8 +20761,11 @@
       <c r="L1" s="34" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
+      <c r="M1" s="20" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>803</v>
       </c>
@@ -20762,7 +20803,7 @@
         <v>3355</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>806</v>
       </c>
@@ -20800,7 +20841,7 @@
         <v>3356</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:13" ht="15.75">
       <c r="A4" s="4" t="s">
         <v>810</v>
       </c>
@@ -20838,7 +20879,7 @@
         <v>3357</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>811</v>
       </c>
@@ -20876,7 +20917,7 @@
         <v>3358</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30.75" customHeight="1">
+    <row r="6" spans="1:13" ht="30.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>816</v>
       </c>
@@ -20914,7 +20955,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>818</v>
       </c>
@@ -20952,7 +20993,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="4" t="s">
         <v>820</v>
       </c>
@@ -20990,7 +21031,7 @@
         <v>3361</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="B9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -21001,7 +21042,7 @@
       <c r="K9" s="22"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="31.5">
+    <row r="10" spans="1:13" ht="31.5">
       <c r="A10" s="4" t="s">
         <v>831</v>
       </c>
@@ -21039,7 +21080,7 @@
         <v>3362</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="63">
+    <row r="11" spans="1:13" ht="63">
       <c r="A11" s="4" t="s">
         <v>835</v>
       </c>
@@ -21077,7 +21118,7 @@
         <v>3363</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="31.5">
+    <row r="12" spans="1:13" ht="31.5">
       <c r="A12" s="4" t="s">
         <v>860</v>
       </c>
@@ -21115,7 +21156,7 @@
         <v>3364</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="31.5">
+    <row r="13" spans="1:13" ht="31.5">
       <c r="A13" s="4" t="s">
         <v>861</v>
       </c>
@@ -21153,7 +21194,7 @@
         <v>3365</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="126">
+    <row r="14" spans="1:13" ht="126">
       <c r="A14" s="4" t="s">
         <v>862</v>
       </c>
@@ -21191,10 +21232,10 @@
         <v>3366</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="K16" s="22"/>
     </row>
     <row r="17" spans="11:11">
@@ -21326,10 +21367,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H12"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21337,15 +21378,15 @@
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="58.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -21382,8 +21423,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>198</v>
       </c>
@@ -21421,7 +21465,7 @@
         <v>3367</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>199</v>
       </c>
@@ -21459,7 +21503,7 @@
         <v>3368</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="75">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" s="4" t="s">
         <v>200</v>
       </c>
@@ -21497,7 +21541,7 @@
         <v>3369</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" s="4" t="s">
         <v>201</v>
       </c>
@@ -21535,7 +21579,7 @@
         <v>3370</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" s="4" t="s">
         <v>202</v>
       </c>
@@ -21573,7 +21617,7 @@
         <v>3371</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" s="4" t="s">
         <v>203</v>
       </c>
@@ -21611,7 +21655,7 @@
         <v>3372</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>204</v>
       </c>
@@ -21649,7 +21693,7 @@
         <v>3373</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="4" t="s">
         <v>205</v>
       </c>
@@ -21687,7 +21731,7 @@
         <v>3374</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>206</v>
       </c>
@@ -21725,7 +21769,7 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
         <v>208</v>
       </c>
@@ -21763,7 +21807,7 @@
         <v>3376</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
         <v>207</v>
       </c>
@@ -21801,7 +21845,7 @@
         <v>3377</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>1836</v>
       </c>
@@ -21824,7 +21868,7 @@
         <v>3378</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>1838</v>
       </c>
@@ -21855,29 +21899,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7" style="4" customWidth="1"/>
     <col min="6" max="6" width="6.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="49.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="4" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="214.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="11" max="11" width="16.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7" style="4" customWidth="1"/>
+    <col min="13" max="13" width="64" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1">
+    <row r="1" spans="1:13" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -21914,8 +21959,11 @@
       <c r="L1" s="34" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="6" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>502</v>
       </c>
@@ -21953,7 +22001,7 @@
         <v>3380</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>504</v>
       </c>
@@ -21991,7 +22039,7 @@
         <v>3381</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>506</v>
       </c>
@@ -22029,7 +22077,7 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
         <v>508</v>
       </c>
@@ -22067,7 +22115,7 @@
         <v>3383</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" s="4" t="s">
         <v>511</v>
       </c>
@@ -22105,7 +22153,7 @@
         <v>3384</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="60">
+    <row r="7" spans="1:13" ht="60">
       <c r="A7" s="4" t="s">
         <v>512</v>
       </c>
@@ -22143,7 +22191,7 @@
         <v>3385</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="4" t="s">
         <v>514</v>
       </c>
@@ -22181,7 +22229,7 @@
         <v>3386</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" s="4" t="s">
         <v>516</v>
       </c>
@@ -22219,7 +22267,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" s="4" t="s">
         <v>692</v>
       </c>
@@ -22257,7 +22305,7 @@
         <v>3388</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
         <v>1315</v>
       </c>
@@ -22292,7 +22340,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
         <v>1318</v>
       </c>
@@ -22327,7 +22375,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="7" t="s">
         <v>1320</v>
       </c>
@@ -22357,7 +22405,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
         <v>1322</v>
       </c>
@@ -22387,7 +22435,7 @@
         <v>3391</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
         <v>1694</v>
       </c>
@@ -22422,7 +22470,7 @@
         <v>3392</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
         <v>1710</v>
       </c>
@@ -23307,27 +23355,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="49" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -23364,8 +23412,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>393</v>
       </c>
@@ -23403,7 +23454,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>398</v>
       </c>
@@ -23441,7 +23492,7 @@
         <v>3418</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>400</v>
       </c>
@@ -23479,7 +23530,7 @@
         <v>3419</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
         <v>404</v>
       </c>
@@ -23517,7 +23568,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>407</v>
       </c>
@@ -23555,7 +23606,7 @@
         <v>3421</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
         <v>410</v>
       </c>
@@ -23593,7 +23644,7 @@
         <v>3422</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="4" t="s">
         <v>412</v>
       </c>
@@ -23631,7 +23682,7 @@
         <v>3423</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="4" t="s">
         <v>415</v>
       </c>
@@ -23669,7 +23720,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>419</v>
       </c>
@@ -23705,7 +23756,7 @@
         <v>3425</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="4" t="s">
         <v>421</v>
       </c>
@@ -23743,7 +23794,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30">
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="4" t="s">
         <v>424</v>
       </c>
@@ -23781,7 +23832,7 @@
         <v>3427</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" s="4" t="s">
         <v>426</v>
       </c>
@@ -23819,7 +23870,7 @@
         <v>3428</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="4" t="s">
         <v>429</v>
       </c>
@@ -23857,7 +23908,7 @@
         <v>3429</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30">
+    <row r="15" spans="1:13" ht="30">
       <c r="A15" s="4" t="s">
         <v>431</v>
       </c>
@@ -23895,7 +23946,7 @@
         <v>3430</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
         <v>434</v>
       </c>
@@ -24506,24 +24557,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="53.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -24560,8 +24611,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>451</v>
       </c>
@@ -24599,7 +24653,7 @@
         <v>3443</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>452</v>
       </c>
@@ -24637,7 +24691,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -24675,7 +24729,7 @@
         <v>3444</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>459</v>
       </c>
@@ -24713,7 +24767,7 @@
         <v>3445</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -24751,7 +24805,7 @@
         <v>3446</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>462</v>
       </c>
@@ -24789,7 +24843,7 @@
         <v>3447</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>467</v>
       </c>
@@ -24827,7 +24881,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>470</v>
       </c>
@@ -24865,7 +24919,7 @@
         <v>3448</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>473</v>
       </c>
@@ -24903,7 +24957,7 @@
         <v>3449</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>475</v>
       </c>
@@ -24948,28 +25002,28 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
-    <col min="2" max="2" width="76.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
-    <col min="5" max="5" width="150.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="54.140625" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="106.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="123.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
     <col min="12" max="12" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -25006,8 +25060,11 @@
       <c r="L1" s="31" t="s">
         <v>3257</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -25045,7 +25102,7 @@
         <v>3451</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:13" ht="30">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -25083,7 +25140,7 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -25121,7 +25178,7 @@
         <v>3453</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -25159,7 +25216,7 @@
         <v>3454</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -25197,7 +25254,7 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -25235,7 +25292,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -25273,7 +25330,7 @@
         <v>3457</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -25311,7 +25368,7 @@
         <v>3458</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -25349,7 +25406,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:13" ht="30">
       <c r="A11" t="s">
         <v>898</v>
       </c>
@@ -25384,7 +25441,7 @@
         <v>3459</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="105">
+    <row r="12" spans="1:13" ht="105">
       <c r="A12" t="s">
         <v>900</v>
       </c>
@@ -25419,7 +25476,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="B13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -25429,7 +25486,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="23"/>
     </row>
-    <row r="14" spans="1:12" ht="60">
+    <row r="14" spans="1:13" ht="60">
       <c r="A14" t="s">
         <v>1638</v>
       </c>
@@ -25464,7 +25521,7 @@
         <v>3461</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30">
+    <row r="15" spans="1:13" ht="30">
       <c r="A15" t="s">
         <v>1639</v>
       </c>
@@ -25499,7 +25556,7 @@
         <v>3462</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30">
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" t="s">
         <v>1640</v>
       </c>

</xml_diff>

<commit_message>
introdotto supporto per 4 macine nel menu prog SE la CPU invia il codice maccina corretto durante il comando #c identificandosi come macchine Brewmatic
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rhea\rheaSRC\gpu-fts-nestle-2019\MenuProgTranslator\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB94156-CD3F-457C-8751-60F462A04203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="801" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4507" uniqueCount="3947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4513" uniqueCount="3953">
   <si>
     <t>LABEL</t>
   </si>
@@ -11891,11 +11892,29 @@
   <si>
     <t>JP</t>
   </si>
+  <si>
+    <t>$LAB_4GRINDER_SETTINGS</t>
+  </si>
+  <si>
+    <t>$LAB_4GRINDER_VIBRATION_SPEED</t>
+  </si>
+  <si>
+    <t>$LAB_4GRINDER_VIBRATION_TIME</t>
+  </si>
+  <si>
+    <t>VIBRATION TIME</t>
+  </si>
+  <si>
+    <t>VIBRATION SPEED</t>
+  </si>
+  <si>
+    <t>VIBRATION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -12395,11 +12414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14956,7 +14975,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
     <sortCondition ref="B2:B47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14965,7 +14984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16276,7 +16295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16375,7 +16394,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30">
+    <row r="3" spans="1:13" ht="60">
       <c r="A3" t="s">
         <v>268</v>
       </c>
@@ -16413,7 +16432,7 @@
         <v>3556</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -16451,7 +16470,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30">
+    <row r="5" spans="1:13" ht="75">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -16489,7 +16508,7 @@
         <v>3558</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45">
+    <row r="6" spans="1:13" ht="90">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -16525,7 +16544,7 @@
         <v>3559</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30">
+    <row r="7" spans="1:13" ht="45">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -16563,7 +16582,7 @@
         <v>3560</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" t="s">
         <v>275</v>
       </c>
@@ -16601,7 +16620,7 @@
         <v>3561</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" t="s">
         <v>278</v>
       </c>
@@ -16639,7 +16658,7 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" t="s">
         <v>280</v>
       </c>
@@ -16677,7 +16696,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30">
+    <row r="11" spans="1:13" ht="75">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -16715,7 +16734,7 @@
         <v>3564</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30">
+    <row r="12" spans="1:13" ht="60">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -16753,7 +16772,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30">
+    <row r="13" spans="1:13" ht="75">
       <c r="A13" t="s">
         <v>292</v>
       </c>
@@ -16791,7 +16810,7 @@
         <v>3566</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30">
+    <row r="14" spans="1:13" ht="60">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -16829,7 +16848,7 @@
         <v>3567</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row r="15" spans="1:13" ht="75">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -16867,7 +16886,7 @@
         <v>3568</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75">
+    <row r="16" spans="1:13" ht="120">
       <c r="A16" t="s">
         <v>301</v>
       </c>
@@ -16905,7 +16924,7 @@
         <v>3569</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30">
+    <row r="17" spans="1:12" ht="60">
       <c r="A17" t="s">
         <v>302</v>
       </c>
@@ -16943,7 +16962,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" t="s">
         <v>590</v>
       </c>
@@ -17014,7 +17033,7 @@
         <v>3572</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="30">
       <c r="A20" t="s">
         <v>842</v>
       </c>
@@ -17090,7 +17109,7 @@
         <v>3574</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" t="s">
         <v>846</v>
       </c>
@@ -17128,7 +17147,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="60">
+    <row r="23" spans="1:12" ht="105">
       <c r="A23" t="s">
         <v>848</v>
       </c>
@@ -17166,7 +17185,7 @@
         <v>3576</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" t="s">
         <v>855</v>
       </c>
@@ -17204,7 +17223,7 @@
         <v>3577</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="45">
+    <row r="25" spans="1:12" ht="75">
       <c r="A25" t="s">
         <v>1572</v>
       </c>
@@ -17234,7 +17253,7 @@
         <v>3578</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="165">
+    <row r="26" spans="1:12" ht="345">
       <c r="A26" t="s">
         <v>1575</v>
       </c>
@@ -17264,7 +17283,7 @@
         <v>3579</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="195">
+    <row r="27" spans="1:12" ht="409.5">
       <c r="A27" t="s">
         <v>1576</v>
       </c>
@@ -17294,7 +17313,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="135">
+    <row r="28" spans="1:12" ht="300">
       <c r="A28" t="s">
         <v>1578</v>
       </c>
@@ -17324,7 +17343,7 @@
         <v>3581</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45">
+    <row r="29" spans="1:12" ht="90">
       <c r="A29" t="s">
         <v>1584</v>
       </c>
@@ -17357,7 +17376,7 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="45">
+    <row r="30" spans="1:12" ht="90">
       <c r="A30" t="s">
         <v>1586</v>
       </c>
@@ -17397,7 +17416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17655,7 +17674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17719,7 +17738,7 @@
         <v>3946</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -17757,7 +17776,7 @@
         <v>3588</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="30">
       <c r="A3" t="s">
         <v>326</v>
       </c>
@@ -17833,7 +17852,7 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" t="s">
         <v>332</v>
       </c>
@@ -17877,7 +17896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18127,7 +18146,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45">
+    <row r="7" spans="1:13" ht="105">
       <c r="A7" s="4" t="s">
         <v>352</v>
       </c>
@@ -18165,7 +18184,7 @@
         <v>3594</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" ht="60">
       <c r="A8" s="4" t="s">
         <v>356</v>
       </c>
@@ -18203,7 +18222,7 @@
         <v>3595</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" s="4" t="s">
         <v>358</v>
       </c>
@@ -18241,7 +18260,7 @@
         <v>3596</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" s="4" t="s">
         <v>359</v>
       </c>
@@ -18279,7 +18298,7 @@
         <v>3597</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="4" t="s">
         <v>364</v>
       </c>
@@ -18317,7 +18336,7 @@
         <v>3598</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" s="4" t="s">
         <v>367</v>
       </c>
@@ -18355,7 +18374,7 @@
         <v>3599</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" ht="45">
       <c r="A13" s="4" t="s">
         <v>371</v>
       </c>
@@ -18393,7 +18412,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="4" t="s">
         <v>373</v>
       </c>
@@ -18431,7 +18450,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="4" t="s">
         <v>380</v>
       </c>
@@ -18469,7 +18488,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="4" t="s">
         <v>385</v>
       </c>
@@ -18507,7 +18526,7 @@
         <v>3601</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="45">
       <c r="A17" s="4" t="s">
         <v>388</v>
       </c>
@@ -18545,7 +18564,7 @@
         <v>3602</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" s="4" t="s">
         <v>722</v>
       </c>
@@ -18583,7 +18602,7 @@
         <v>3603</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="60">
       <c r="A19" s="4" t="s">
         <v>725</v>
       </c>
@@ -18627,7 +18646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18960,7 +18979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -20068,7 +20087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20701,7 +20720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20955,7 +20974,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75">
+    <row r="7" spans="1:13" ht="120">
       <c r="A7" s="4" t="s">
         <v>818</v>
       </c>
@@ -20993,7 +21012,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75">
+    <row r="8" spans="1:13" ht="105">
       <c r="A8" s="4" t="s">
         <v>820</v>
       </c>
@@ -21042,7 +21061,7 @@
       <c r="K9" s="22"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:13" ht="31.5">
+    <row r="10" spans="1:13" ht="240">
       <c r="A10" s="4" t="s">
         <v>831</v>
       </c>
@@ -21080,7 +21099,7 @@
         <v>3362</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63">
+    <row r="11" spans="1:13" ht="409.5">
       <c r="A11" s="4" t="s">
         <v>835</v>
       </c>
@@ -21118,7 +21137,7 @@
         <v>3363</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31.5">
+    <row r="12" spans="1:13" ht="195">
       <c r="A12" s="4" t="s">
         <v>860</v>
       </c>
@@ -21156,7 +21175,7 @@
         <v>3364</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31.5">
+    <row r="13" spans="1:13" ht="210">
       <c r="A13" s="4" t="s">
         <v>861</v>
       </c>
@@ -21194,7 +21213,7 @@
         <v>3365</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="126">
+    <row r="14" spans="1:13" ht="409.5">
       <c r="A14" s="4" t="s">
         <v>862</v>
       </c>
@@ -21366,7 +21385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -21769,7 +21788,7 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="120">
       <c r="A11" s="4" t="s">
         <v>208</v>
       </c>
@@ -21898,7 +21917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22153,7 +22172,7 @@
         <v>3384</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="60">
+    <row r="7" spans="1:13" ht="210">
       <c r="A7" s="4" t="s">
         <v>512</v>
       </c>
@@ -22405,7 +22424,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="4" t="s">
         <v>1322</v>
       </c>
@@ -22435,7 +22454,7 @@
         <v>3391</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="150">
       <c r="A15" s="4" t="s">
         <v>1694</v>
       </c>
@@ -22470,7 +22489,7 @@
         <v>3392</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="4" t="s">
         <v>1710</v>
       </c>
@@ -22505,7 +22524,7 @@
         <v>3393</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="4" t="s">
         <v>1695</v>
       </c>
@@ -22540,7 +22559,7 @@
         <v>3394</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="4" t="s">
         <v>1697</v>
       </c>
@@ -22575,7 +22594,7 @@
         <v>3395</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="90">
       <c r="A19" s="4" t="s">
         <v>1699</v>
       </c>
@@ -22610,7 +22629,7 @@
         <v>3396</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="75">
       <c r="A20" s="4" t="s">
         <v>1701</v>
       </c>
@@ -22645,7 +22664,7 @@
         <v>3397</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="75">
       <c r="A21" s="4" t="s">
         <v>1703</v>
       </c>
@@ -22680,7 +22699,7 @@
         <v>3398</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="135">
       <c r="A22" s="4" t="s">
         <v>1713</v>
       </c>
@@ -22715,7 +22734,7 @@
         <v>3399</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="75">
       <c r="A23" s="4" t="s">
         <v>1724</v>
       </c>
@@ -22750,7 +22769,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="90">
       <c r="A24" s="4" t="s">
         <v>1727</v>
       </c>
@@ -22785,7 +22804,7 @@
         <v>3401</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="45">
       <c r="A25" s="4" t="s">
         <v>1732</v>
       </c>
@@ -22820,7 +22839,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="45">
       <c r="A26" s="4" t="s">
         <v>1735</v>
       </c>
@@ -22855,7 +22874,7 @@
         <v>3402</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="45">
       <c r="A27" s="4" t="s">
         <v>1740</v>
       </c>
@@ -22883,7 +22902,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="45">
       <c r="A28" s="4" t="s">
         <v>1741</v>
       </c>
@@ -22911,7 +22930,7 @@
         <v>3403</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30">
+    <row r="29" spans="1:12" ht="150">
       <c r="A29" s="4" t="s">
         <v>1742</v>
       </c>
@@ -22941,7 +22960,7 @@
         <v>3404</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="75">
+    <row r="30" spans="1:12" ht="409.5">
       <c r="A30" s="4" t="s">
         <v>1744</v>
       </c>
@@ -22976,7 +22995,7 @@
         <v>3405</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30">
+    <row r="31" spans="1:12" ht="300">
       <c r="A31" s="4" t="s">
         <v>1747</v>
       </c>
@@ -23011,7 +23030,7 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="135">
       <c r="A32" s="4" t="s">
         <v>1750</v>
       </c>
@@ -23046,7 +23065,7 @@
         <v>3407</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" ht="90">
       <c r="A33" s="4" t="s">
         <v>1751</v>
       </c>
@@ -23081,7 +23100,7 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30">
+    <row r="34" spans="1:12" ht="285">
       <c r="A34" s="4" t="s">
         <v>1752</v>
       </c>
@@ -23116,7 +23135,7 @@
         <v>3409</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30">
+    <row r="35" spans="1:12" ht="270">
       <c r="A35" s="4" t="s">
         <v>1753</v>
       </c>
@@ -23149,7 +23168,7 @@
         <v>3410</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="75">
+    <row r="36" spans="1:12" ht="409.5">
       <c r="A36" s="4" t="s">
         <v>1754</v>
       </c>
@@ -23184,7 +23203,7 @@
         <v>3411</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" ht="210">
       <c r="A37" s="4" t="s">
         <v>1756</v>
       </c>
@@ -23219,7 +23238,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30">
+    <row r="38" spans="1:12" ht="405">
       <c r="A38" s="4" t="s">
         <v>1757</v>
       </c>
@@ -23254,7 +23273,7 @@
         <v>3413</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30">
+    <row r="39" spans="1:12" ht="195">
       <c r="A39" s="4" t="s">
         <v>1759</v>
       </c>
@@ -23289,7 +23308,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" ht="165">
       <c r="A40" s="4" t="s">
         <v>1776</v>
       </c>
@@ -23318,7 +23337,7 @@
         <v>3415</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" ht="150">
       <c r="A41" s="4" t="s">
         <v>1774</v>
       </c>
@@ -23354,11 +23373,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23756,7 +23775,7 @@
         <v>3425</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45">
+    <row r="11" spans="1:13" ht="105">
       <c r="A11" s="4" t="s">
         <v>421</v>
       </c>
@@ -23794,7 +23813,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30">
+    <row r="12" spans="1:13" ht="120">
       <c r="A12" s="4" t="s">
         <v>424</v>
       </c>
@@ -23832,7 +23851,7 @@
         <v>3427</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30">
+    <row r="13" spans="1:13" ht="150">
       <c r="A13" s="4" t="s">
         <v>426</v>
       </c>
@@ -23870,7 +23889,7 @@
         <v>3428</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30">
+    <row r="14" spans="1:13" ht="135">
       <c r="A14" s="4" t="s">
         <v>429</v>
       </c>
@@ -23908,7 +23927,7 @@
         <v>3429</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row r="15" spans="1:13" ht="195">
       <c r="A15" s="4" t="s">
         <v>431</v>
       </c>
@@ -23984,7 +24003,7 @@
         <v>3431</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="60">
       <c r="A17" s="4" t="s">
         <v>437</v>
       </c>
@@ -24022,7 +24041,7 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="60">
+    <row r="18" spans="1:12" ht="270">
       <c r="A18" s="4" t="s">
         <v>440</v>
       </c>
@@ -24060,7 +24079,7 @@
         <v>3433</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="60">
       <c r="A19" s="4" t="s">
         <v>442</v>
       </c>
@@ -24098,7 +24117,7 @@
         <v>3434</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="30">
+    <row r="20" spans="1:12" ht="150">
       <c r="A20" s="4" t="s">
         <v>449</v>
       </c>
@@ -24136,7 +24155,7 @@
         <v>3435</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="105">
       <c r="A21" s="4" t="s">
         <v>870</v>
       </c>
@@ -24172,7 +24191,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="75">
       <c r="A22" s="4" t="s">
         <v>873</v>
       </c>
@@ -24208,7 +24227,7 @@
         <v>3437</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="30">
       <c r="A23" s="4" t="s">
         <v>875</v>
       </c>
@@ -24242,7 +24261,7 @@
         <v>3438</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="135">
       <c r="A24" s="4" t="s">
         <v>877</v>
       </c>
@@ -24278,7 +24297,7 @@
         <v>3439</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="105">
       <c r="A25" s="4" t="s">
         <v>880</v>
       </c>
@@ -24314,7 +24333,7 @@
         <v>3440</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="90">
+    <row r="26" spans="1:12" ht="409.5">
       <c r="A26" s="4" t="s">
         <v>884</v>
       </c>
@@ -24350,7 +24369,7 @@
         <v>3441</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30">
+    <row r="27" spans="1:12" ht="165">
       <c r="A27" s="4" t="s">
         <v>889</v>
       </c>
@@ -24403,12 +24422,30 @@
       <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>3949</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>3950</v>
+      </c>
       <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:12">
+      <c r="A31" s="4" t="s">
+        <v>3948</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>3951</v>
+      </c>
       <c r="K31" s="22"/>
     </row>
     <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>3947</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>3952</v>
+      </c>
       <c r="K32" s="22"/>
     </row>
     <row r="33" spans="11:11">
@@ -24556,7 +24593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25001,7 +25038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25064,7 +25101,7 @@
         <v>3946</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -25102,7 +25139,7 @@
         <v>3451</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30">
+    <row r="3" spans="1:13" ht="60">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -25140,7 +25177,7 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -25178,7 +25215,7 @@
         <v>3453</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -25216,7 +25253,7 @@
         <v>3454</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -25254,7 +25291,7 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -25292,7 +25329,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -25330,7 +25367,7 @@
         <v>3457</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -25368,7 +25405,7 @@
         <v>3458</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30">
+    <row r="10" spans="1:13" ht="60">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -25406,7 +25443,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30">
+    <row r="11" spans="1:13" ht="60">
       <c r="A11" t="s">
         <v>898</v>
       </c>
@@ -25441,7 +25478,7 @@
         <v>3459</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="105">
+    <row r="12" spans="1:13" ht="285">
       <c r="A12" t="s">
         <v>900</v>
       </c>
@@ -25486,7 +25523,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="60">
+    <row r="14" spans="1:13" ht="90">
       <c r="A14" t="s">
         <v>1638</v>
       </c>
@@ -25521,7 +25558,7 @@
         <v>3461</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row r="15" spans="1:13" ht="60">
       <c r="A15" t="s">
         <v>1639</v>
       </c>
@@ -25556,7 +25593,7 @@
         <v>3462</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30">
+    <row r="16" spans="1:13" ht="60">
       <c r="A16" t="s">
         <v>1640</v>
       </c>
@@ -25591,7 +25628,7 @@
         <v>3463</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30">
+    <row r="17" spans="1:12" ht="60">
       <c r="A17" t="s">
         <v>1641</v>
       </c>
@@ -25661,7 +25698,7 @@
         <v>3465</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30">
+    <row r="19" spans="1:12" ht="60">
       <c r="A19" t="s">
         <v>1643</v>
       </c>
@@ -25731,7 +25768,7 @@
         <v>3467</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="60">
+    <row r="21" spans="1:12" ht="75">
       <c r="A21" t="s">
         <v>1645</v>
       </c>
@@ -25766,7 +25803,7 @@
         <v>3468</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30">
+    <row r="22" spans="1:12" ht="75">
       <c r="A22" t="s">
         <v>1646</v>
       </c>
@@ -25801,7 +25838,7 @@
         <v>3469</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="30">
       <c r="A23" t="s">
         <v>1647</v>
       </c>
@@ -25951,7 +25988,7 @@
         <v>3473</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="30">
+    <row r="28" spans="1:12" ht="45">
       <c r="A28" t="s">
         <v>1606</v>
       </c>
@@ -25986,7 +26023,7 @@
         <v>3474</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30">
+    <row r="29" spans="1:12" ht="45">
       <c r="A29" t="s">
         <v>1607</v>
       </c>
@@ -26056,7 +26093,7 @@
         <v>3476</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30">
+    <row r="31" spans="1:12" ht="60">
       <c r="A31" t="s">
         <v>1609</v>
       </c>
@@ -26133,7 +26170,7 @@
         <v>3478</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="45">
+    <row r="34" spans="1:12" ht="105">
       <c r="A34" t="s">
         <v>1651</v>
       </c>
@@ -26165,7 +26202,7 @@
         <v>3479</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" ht="30">
       <c r="A35" t="s">
         <v>1652</v>
       </c>
@@ -26197,7 +26234,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30">
+    <row r="36" spans="1:12" ht="60">
       <c r="A36" t="s">
         <v>1653</v>
       </c>
@@ -26229,7 +26266,7 @@
         <v>3481</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="45">
+    <row r="37" spans="1:12" ht="60">
       <c r="A37" t="s">
         <v>1654</v>
       </c>
@@ -26261,7 +26298,7 @@
         <v>3482</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30">
+    <row r="38" spans="1:12" ht="60">
       <c r="A38" t="s">
         <v>1655</v>
       </c>
@@ -26293,7 +26330,7 @@
         <v>3483</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30">
+    <row r="39" spans="1:12" ht="45">
       <c r="A39" t="s">
         <v>1662</v>
       </c>
@@ -26421,7 +26458,7 @@
         <v>3487</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30">
+    <row r="43" spans="1:12" ht="60">
       <c r="A43" t="s">
         <v>1650</v>
       </c>
@@ -26453,7 +26490,7 @@
         <v>3488</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30">
+    <row r="44" spans="1:12" ht="75">
       <c r="A44" t="s">
         <v>1659</v>
       </c>
@@ -26485,7 +26522,7 @@
         <v>3489</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="60">
+    <row r="45" spans="1:12" ht="120">
       <c r="A45" t="s">
         <v>1660</v>
       </c>
@@ -26517,7 +26554,7 @@
         <v>3490</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30">
+    <row r="46" spans="1:12" ht="45">
       <c r="A46" t="s">
         <v>1663</v>
       </c>
@@ -26733,7 +26770,7 @@
         <v>3497</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="30">
+    <row r="53" spans="1:12" ht="60">
       <c r="A53" t="s">
         <v>1676</v>
       </c>
@@ -26765,7 +26802,7 @@
         <v>3498</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="30">
+    <row r="54" spans="1:12" ht="60">
       <c r="A54" t="s">
         <v>1678</v>
       </c>
@@ -26797,7 +26834,7 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30">
+    <row r="55" spans="1:12" ht="60">
       <c r="A55" t="s">
         <v>1687</v>
       </c>
@@ -26829,7 +26866,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" ht="45">
       <c r="A56" t="s">
         <v>1689</v>
       </c>
@@ -26861,7 +26898,7 @@
         <v>3501</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" ht="30">
       <c r="A57" t="s">
         <v>1690</v>
       </c>
@@ -26893,7 +26930,7 @@
         <v>3502</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" ht="30">
       <c r="A58" t="s">
         <v>1691</v>
       </c>
@@ -26925,7 +26962,7 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" ht="30">
       <c r="A59" t="s">
         <v>1692</v>
       </c>
@@ -26957,7 +26994,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="75">
+    <row r="60" spans="1:12" ht="120">
       <c r="A60" t="s">
         <v>1693</v>
       </c>
@@ -27000,7 +27037,7 @@
       <c r="K61" s="19"/>
       <c r="L61" s="23"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" ht="45">
       <c r="A62" t="s">
         <v>1788</v>
       </c>
@@ -27035,7 +27072,7 @@
         <v>3506</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="45">
+    <row r="63" spans="1:12" ht="60">
       <c r="A63" t="s">
         <v>1787</v>
       </c>
@@ -27070,7 +27107,7 @@
         <v>3507</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="105">
+    <row r="64" spans="1:12" ht="210">
       <c r="A64" t="s">
         <v>1829</v>
       </c>
@@ -27105,7 +27142,7 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30">
+    <row r="65" spans="1:12" ht="60">
       <c r="A65" t="s">
         <v>1786</v>
       </c>
@@ -27140,7 +27177,7 @@
         <v>3509</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="30">
+    <row r="66" spans="1:12" ht="90">
       <c r="A66" t="s">
         <v>1793</v>
       </c>
@@ -27175,7 +27212,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" ht="30">
       <c r="A67" t="s">
         <v>1795</v>
       </c>
@@ -27210,7 +27247,7 @@
         <v>3511</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="60">
+    <row r="68" spans="1:12" ht="105">
       <c r="A68" t="s">
         <v>1800</v>
       </c>
@@ -27245,7 +27282,7 @@
         <v>3512</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="45">
+    <row r="69" spans="1:12" ht="90">
       <c r="A69" t="s">
         <v>1797</v>
       </c>
@@ -27280,7 +27317,7 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="30">
+    <row r="70" spans="1:12" ht="60">
       <c r="A70" t="s">
         <v>1804</v>
       </c>
@@ -27315,7 +27352,7 @@
         <v>3514</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="30">
+    <row r="71" spans="1:12" ht="75">
       <c r="A71" t="s">
         <v>1799</v>
       </c>
@@ -27350,7 +27387,7 @@
         <v>3515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="75">
+    <row r="72" spans="1:12" ht="150">
       <c r="A72" t="s">
         <v>1806</v>
       </c>
@@ -27385,7 +27422,7 @@
         <v>3516</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="30">
+    <row r="73" spans="1:12" ht="45">
       <c r="A73" t="s">
         <v>1808</v>
       </c>
@@ -27420,7 +27457,7 @@
         <v>3517</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="30">
+    <row r="74" spans="1:12" ht="60">
       <c r="A74" t="s">
         <v>1810</v>
       </c>
@@ -27455,7 +27492,7 @@
         <v>3518</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="30">
+    <row r="75" spans="1:12" ht="60">
       <c r="A75" t="s">
         <v>1812</v>
       </c>
@@ -27490,7 +27527,7 @@
         <v>3519</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="30">
+    <row r="76" spans="1:12" ht="45">
       <c r="A76" t="s">
         <v>1814</v>
       </c>
@@ -27525,7 +27562,7 @@
         <v>3520</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" ht="45">
       <c r="A77" t="s">
         <v>1816</v>
       </c>
@@ -27560,7 +27597,7 @@
         <v>3521</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="30">
+    <row r="78" spans="1:12" ht="45">
       <c r="A78" t="s">
         <v>1817</v>
       </c>

</xml_diff>

<commit_message>
Aggiunta voce "CUP SIZE" in ogni selezione del menu prog
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbrunelli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rhea\rheaSRC\gpu-fts-nestle-2019\MenuProgTranslator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="14"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4905" uniqueCount="4333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="4335">
   <si>
     <t>LABEL</t>
   </si>
@@ -13503,6 +13503,12 @@
   </si>
   <si>
     <t>Wilt u de maalhandelingen herhalen?</t>
+  </si>
+  <si>
+    <t>$LAB_SEL_CUP_SIZE</t>
+  </si>
+  <si>
+    <t>CUP SIZE</t>
   </si>
 </sst>
 </file>
@@ -14143,7 +14149,7 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16920,10 +16926,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -18323,6 +18329,14 @@
       </c>
       <c r="M34" s="33" t="s">
         <v>4261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A35" t="s">
+        <v>4333</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>4334</v>
       </c>
     </row>
   </sheetData>
@@ -20858,7 +20872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -22394,9 +22408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
@@ -23779,7 +23791,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -24292,7 +24304,7 @@
       <c r="A13" t="s">
         <v>1836</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>1837</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -27753,7 +27765,7 @@
   <dimension ref="A1:M108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M108"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
mantengo l'lallineamento del file di lingue tra i 3 rami attualmenti aperti (develop, brewmatic, rhTT)
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rhea\rheaSRC\gpu-fts-nestle-2019\MenuProgTranslator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbrunelli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4905" uniqueCount="4333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="4335">
   <si>
     <t>LABEL</t>
   </si>
@@ -13503,6 +13503,12 @@
   </si>
   <si>
     <t>Wilt u de maalhandelingen herhalen?</t>
+  </si>
+  <si>
+    <t>$LAB_SEL_CUP_SIZE</t>
+  </si>
+  <si>
+    <t>CUP SIZE</t>
   </si>
 </sst>
 </file>
@@ -14142,8 +14148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16920,10 +16926,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -18323,6 +18329,14 @@
       </c>
       <c r="M34" s="33" t="s">
         <v>4261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A35" t="s">
+        <v>4333</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>4334</v>
       </c>
     </row>
   </sheetData>
@@ -22394,9 +22408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
@@ -23779,7 +23791,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -24292,7 +24304,7 @@
       <c r="A13" t="s">
         <v>1836</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>1837</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -27753,7 +27765,7 @@
   <dimension ref="A1:M108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M108"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Aggiunto pulsante "TEST VIBRATION" in menu prog > DEVICES > OTHER per testare lo scivolo vibrante di Brewmatic. Il pulsante è visible solo se CPU riporta come codice macchia "brewmatic". Passo a Linux per compilazione
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="9"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="4335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4909" uniqueCount="4337">
   <si>
     <t>LABEL</t>
   </si>
@@ -13509,6 +13509,12 @@
   </si>
   <si>
     <t>CUP SIZE</t>
+  </si>
+  <si>
+    <t>$LAB_STOP</t>
+  </si>
+  <si>
+    <t>STOP</t>
   </si>
 </sst>
 </file>
@@ -14146,10 +14152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16463,327 +16469,303 @@
     </row>
     <row r="58" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A58" t="s">
-        <v>497</v>
+        <v>4335</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>498</v>
-      </c>
-      <c r="C58" t="s">
-        <v>499</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>644</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>995</v>
-      </c>
-      <c r="F58" t="s">
-        <v>995</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>1378</v>
-      </c>
-      <c r="H58" s="21" t="s">
-        <v>1957</v>
-      </c>
-      <c r="I58" s="18" t="s">
-        <v>3653</v>
-      </c>
-      <c r="J58" s="18" t="s">
-        <v>2298</v>
-      </c>
-      <c r="K58" s="18" t="s">
-        <v>2964</v>
-      </c>
-      <c r="L58" s="18" t="s">
-        <v>3309</v>
-      </c>
-      <c r="M58" s="33" t="s">
-        <v>3999</v>
-      </c>
+        <v>4336</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="18"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="36"/>
     </row>
     <row r="59" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A59" t="s">
+        <v>497</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="C59" t="s">
+        <v>499</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>644</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>995</v>
+      </c>
+      <c r="F59" t="s">
+        <v>995</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>1957</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>3653</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>2298</v>
+      </c>
+      <c r="K59" s="18" t="s">
+        <v>2964</v>
+      </c>
+      <c r="L59" s="18" t="s">
+        <v>3309</v>
+      </c>
+      <c r="M59" s="33" t="s">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A60" t="s">
         <v>209</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B60" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>211</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="D60" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>996</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>1379</v>
       </c>
-      <c r="H59" s="21" t="s">
+      <c r="H60" s="21" t="s">
         <v>1958</v>
       </c>
-      <c r="I59" s="18" t="s">
+      <c r="I60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="J59" s="18" t="s">
+      <c r="J60" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="K59" s="18" t="s">
+      <c r="K60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="L59" s="18" t="s">
+      <c r="L60" s="18" t="s">
         <v>3310</v>
       </c>
-      <c r="M59" s="34" t="s">
+      <c r="M60" s="34" t="s">
         <v>4000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>997</v>
-      </c>
-      <c r="F60" t="s">
-        <v>998</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>1380</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>1959</v>
-      </c>
-      <c r="I60" s="18" t="s">
-        <v>3654</v>
-      </c>
-      <c r="J60" s="18" t="s">
-        <v>2299</v>
-      </c>
-      <c r="K60" s="18" t="s">
-        <v>2299</v>
-      </c>
-      <c r="L60" s="18" t="s">
-        <v>3311</v>
-      </c>
-      <c r="M60" s="36" t="s">
-        <v>4001</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>490</v>
+        <v>96</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>488</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>489</v>
+        <v>98</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>645</v>
+        <v>97</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F61" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="K61" s="18" t="s">
-        <v>2965</v>
+        <v>2299</v>
       </c>
       <c r="L61" s="18" t="s">
-        <v>3312</v>
-      </c>
-      <c r="M61" s="33" t="s">
-        <v>4002</v>
+        <v>3311</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>4001</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="C62" t="s">
+        <v>489</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>999</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>1381</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>1960</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>3655</v>
+      </c>
+      <c r="J62" s="18" t="s">
+        <v>2300</v>
+      </c>
+      <c r="K62" s="18" t="s">
+        <v>2965</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>3312</v>
+      </c>
+      <c r="M62" s="33" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A63" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>482</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>484</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E63" s="18" t="s">
         <v>1001</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>1002</v>
       </c>
-      <c r="G62" s="8" t="s">
+      <c r="G63" s="8" t="s">
         <v>1382</v>
       </c>
-      <c r="H62" s="21" t="s">
+      <c r="H63" s="21" t="s">
         <v>1961</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I63" s="18" t="s">
         <v>3656</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J63" s="18" t="s">
         <v>2301</v>
       </c>
-      <c r="K62" s="18" t="s">
+      <c r="K63" s="18" t="s">
         <v>2966</v>
       </c>
-      <c r="L62" s="18" t="s">
+      <c r="L63" s="18" t="s">
         <v>3313</v>
       </c>
-      <c r="M62" s="33" t="s">
+      <c r="M63" s="33" t="s">
         <v>4003</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A63" t="s">
+    <row r="64" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A64" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B64" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>58</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>647</v>
       </c>
-      <c r="E63" s="18" t="s">
+      <c r="E64" s="18" t="s">
         <v>1003</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>1004</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G64" s="8" t="s">
         <v>1383</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H64" s="21" t="s">
         <v>1962</v>
       </c>
-      <c r="I63" s="18" t="s">
+      <c r="I64" s="18" t="s">
         <v>3657</v>
       </c>
-      <c r="J63" s="18" t="s">
+      <c r="J64" s="18" t="s">
         <v>2302</v>
       </c>
-      <c r="K63" s="18" t="s">
+      <c r="K64" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="L63" s="18" t="s">
+      <c r="L64" s="18" t="s">
         <v>3314</v>
       </c>
-      <c r="M63" s="33" t="s">
+      <c r="M64" s="33" t="s">
         <v>4004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A64" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C64" t="s">
-        <v>155</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>648</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1005</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>1384</v>
-      </c>
-      <c r="H64" s="21" t="s">
-        <v>1963</v>
-      </c>
-      <c r="I64" s="18" t="s">
-        <v>3658</v>
-      </c>
-      <c r="J64" s="18" t="s">
-        <v>2303</v>
-      </c>
-      <c r="K64" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="L64" s="18" t="s">
-        <v>3315</v>
-      </c>
-      <c r="M64" s="36" t="s">
-        <v>4005</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F65" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>1384</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="I65" s="18" t="s">
         <v>3658</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="K65" s="18" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>3316</v>
+        <v>3315</v>
       </c>
       <c r="M65" s="36" t="s">
         <v>4005</v>
@@ -16791,127 +16773,168 @@
     </row>
     <row r="66" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>486</v>
+        <v>106</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>485</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>487</v>
+        <v>105</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F66" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="K66" s="18" t="s">
-        <v>2967</v>
+        <v>104</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>3317</v>
-      </c>
-      <c r="M66" s="33" t="s">
-        <v>4006</v>
+        <v>3316</v>
+      </c>
+      <c r="M66" s="36" t="s">
+        <v>4005</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>36</v>
+        <v>486</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>37</v>
+        <v>485</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>487</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>38</v>
+        <v>1007</v>
       </c>
       <c r="F67" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>2968</v>
+        <v>3659</v>
       </c>
       <c r="J67" s="18" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="K67" s="18" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>3318</v>
+        <v>3317</v>
       </c>
       <c r="M67" s="33" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>1855</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1854</v>
+        <v>36</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>1856</v>
+        <v>38</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>1857</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>1858</v>
+        <v>600</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>1386</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>1966</v>
+      </c>
+      <c r="I68" s="18" t="s">
+        <v>2968</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>2306</v>
+      </c>
+      <c r="K68" s="18" t="s">
+        <v>2968</v>
+      </c>
+      <c r="L68" s="18" t="s">
+        <v>3318</v>
       </c>
       <c r="M68" s="33" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>1900</v>
+        <v>1855</v>
       </c>
       <c r="B69" t="s">
-        <v>1901</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="M69" s="35" t="s">
-        <v>4009</v>
+        <v>1854</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>1857</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>1858</v>
+      </c>
+      <c r="M69" s="33" t="s">
+        <v>4008</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="B70" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="D70" s="27"/>
       <c r="M70" s="35" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="3" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D71" s="27"/>
+      <c r="M71" s="35" t="s">
         <v>4010</v>
       </c>
     </row>
@@ -16928,7 +16951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -25978,8 +26001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
modificati alcuni parametri in MILKER > CAPPINDUX relativi ai minimi e massimi valori ammissibil per i template del capp
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4909" uniqueCount="4337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="4349">
   <si>
     <t>LABEL</t>
   </si>
@@ -13515,6 +13515,42 @@
   </si>
   <si>
     <t>STOP</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H1</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H2</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H3</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C1</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C2</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C3</t>
+  </si>
+  <si>
+    <t>HOT CLASSIC FOAM</t>
+  </si>
+  <si>
+    <t>HOT FLUFFY FOAM</t>
+  </si>
+  <si>
+    <t>HOT BARISTA FOAM</t>
+  </si>
+  <si>
+    <t>COLD CLASSIC FOAM</t>
+  </si>
+  <si>
+    <t>COLD FLUFFY FOAM</t>
+  </si>
+  <si>
+    <t>COLD BARISTA FOAM</t>
   </si>
 </sst>
 </file>
@@ -14154,7 +14190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -24383,16 +24419,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="37" style="4" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" customWidth="1"/>
     <col min="5" max="5" width="7" style="4" customWidth="1"/>
@@ -25989,6 +26025,54 @@
       </c>
       <c r="M41" s="40" t="s">
         <v>4108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="4" t="s">
+        <v>4337</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="4" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>4339</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>4340</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="4" t="s">
+        <v>4341</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="4" t="s">
+        <v>4342</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>4348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primi lavori per supporto SNACK
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="5"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="4349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4925" uniqueCount="4353">
   <si>
     <t>LABEL</t>
   </si>
@@ -13551,6 +13551,18 @@
   </si>
   <si>
     <t>COLD BARISTA FOAM</t>
+  </si>
+  <si>
+    <t>$LAB_ENTER_PROG</t>
+  </si>
+  <si>
+    <t>ENTER PROGRAMMING</t>
+  </si>
+  <si>
+    <t>$LAB_EXIT_PROG</t>
+  </si>
+  <si>
+    <t>EXIT PROGRAMMING</t>
   </si>
 </sst>
 </file>
@@ -14188,10 +14200,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16972,6 +16984,22 @@
       <c r="D71" s="27"/>
       <c r="M71" s="35" t="s">
         <v>4010</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A72" s="3" t="s">
+        <v>4349</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A73" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4352</v>
       </c>
     </row>
   </sheetData>
@@ -24421,7 +24449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -26085,7 +26113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggiunta voce "DETECTED CUP SIZE" in menu prog > DEVICE > OTHER in luogo di CUP THRESHOLD nel caso di macchine Brewmatic
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4925" uniqueCount="4353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4929" uniqueCount="4357">
   <si>
     <t>LABEL</t>
   </si>
@@ -13563,6 +13563,18 @@
   </si>
   <si>
     <t>EXIT PROGRAMMING</t>
+  </si>
+  <si>
+    <t>$LAB_DEV_CUP_SIZE_DETECTED</t>
+  </si>
+  <si>
+    <t>DETECTED CUP SIZE</t>
+  </si>
+  <si>
+    <t>$LAB_DEV_NO_CUP_DETECTED</t>
+  </si>
+  <si>
+    <t>NO CUP DETECTED</t>
   </si>
 </sst>
 </file>
@@ -14202,7 +14214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -18434,15 +18446,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -19633,6 +19645,22 @@
       </c>
       <c r="M30" s="33" t="s">
         <v>4289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>4353</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>4355</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>4356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunte label traduzioni per nuova voce menu prog device detected cup
</commit_message>
<xml_diff>
--- a/MenuProgTranslator/translations.xlsx
+++ b/MenuProgTranslator/translations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbrunelli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rhea\rheaSRC\gpu-fts-nestle-2019\MenuProgTranslator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="9"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="uso comune" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="4335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4929" uniqueCount="4357">
   <si>
     <t>LABEL</t>
   </si>
@@ -13509,6 +13509,72 @@
   </si>
   <si>
     <t>CUP SIZE</t>
+  </si>
+  <si>
+    <t>$LAB_STOP</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H1</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H2</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_H3</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C1</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C2</t>
+  </si>
+  <si>
+    <t>$LAB_MILKER2_TEMPLATE_C3</t>
+  </si>
+  <si>
+    <t>HOT CLASSIC FOAM</t>
+  </si>
+  <si>
+    <t>HOT FLUFFY FOAM</t>
+  </si>
+  <si>
+    <t>HOT BARISTA FOAM</t>
+  </si>
+  <si>
+    <t>COLD CLASSIC FOAM</t>
+  </si>
+  <si>
+    <t>COLD FLUFFY FOAM</t>
+  </si>
+  <si>
+    <t>COLD BARISTA FOAM</t>
+  </si>
+  <si>
+    <t>$LAB_ENTER_PROG</t>
+  </si>
+  <si>
+    <t>ENTER PROGRAMMING</t>
+  </si>
+  <si>
+    <t>$LAB_EXIT_PROG</t>
+  </si>
+  <si>
+    <t>EXIT PROGRAMMING</t>
+  </si>
+  <si>
+    <t>$LAB_DEV_CUP_SIZE_DETECTED</t>
+  </si>
+  <si>
+    <t>DETECTED CUP SIZE</t>
+  </si>
+  <si>
+    <t>$LAB_DEV_NO_CUP_DETECTED</t>
+  </si>
+  <si>
+    <t>NO CUP DETECTED</t>
   </si>
 </sst>
 </file>
@@ -14146,10 +14212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -16463,327 +16529,303 @@
     </row>
     <row r="58" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A58" t="s">
-        <v>497</v>
+        <v>4335</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>498</v>
-      </c>
-      <c r="C58" t="s">
-        <v>499</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>644</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>995</v>
-      </c>
-      <c r="F58" t="s">
-        <v>995</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>1378</v>
-      </c>
-      <c r="H58" s="21" t="s">
-        <v>1957</v>
-      </c>
-      <c r="I58" s="18" t="s">
-        <v>3653</v>
-      </c>
-      <c r="J58" s="18" t="s">
-        <v>2298</v>
-      </c>
-      <c r="K58" s="18" t="s">
-        <v>2964</v>
-      </c>
-      <c r="L58" s="18" t="s">
-        <v>3309</v>
-      </c>
-      <c r="M58" s="33" t="s">
-        <v>3999</v>
-      </c>
+        <v>4336</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="18"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="36"/>
     </row>
     <row r="59" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A59" t="s">
+        <v>497</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="C59" t="s">
+        <v>499</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>644</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>995</v>
+      </c>
+      <c r="F59" t="s">
+        <v>995</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>1957</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>3653</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>2298</v>
+      </c>
+      <c r="K59" s="18" t="s">
+        <v>2964</v>
+      </c>
+      <c r="L59" s="18" t="s">
+        <v>3309</v>
+      </c>
+      <c r="M59" s="33" t="s">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A60" t="s">
         <v>209</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B60" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>211</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="D60" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>996</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>1379</v>
       </c>
-      <c r="H59" s="21" t="s">
+      <c r="H60" s="21" t="s">
         <v>1958</v>
       </c>
-      <c r="I59" s="18" t="s">
+      <c r="I60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="J59" s="18" t="s">
+      <c r="J60" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="K59" s="18" t="s">
+      <c r="K60" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="L59" s="18" t="s">
+      <c r="L60" s="18" t="s">
         <v>3310</v>
       </c>
-      <c r="M59" s="34" t="s">
+      <c r="M60" s="34" t="s">
         <v>4000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>997</v>
-      </c>
-      <c r="F60" t="s">
-        <v>998</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>1380</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>1959</v>
-      </c>
-      <c r="I60" s="18" t="s">
-        <v>3654</v>
-      </c>
-      <c r="J60" s="18" t="s">
-        <v>2299</v>
-      </c>
-      <c r="K60" s="18" t="s">
-        <v>2299</v>
-      </c>
-      <c r="L60" s="18" t="s">
-        <v>3311</v>
-      </c>
-      <c r="M60" s="36" t="s">
-        <v>4001</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>490</v>
+        <v>96</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>488</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>489</v>
+        <v>98</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>645</v>
+        <v>97</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F61" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="K61" s="18" t="s">
-        <v>2965</v>
+        <v>2299</v>
       </c>
       <c r="L61" s="18" t="s">
-        <v>3312</v>
-      </c>
-      <c r="M61" s="33" t="s">
-        <v>4002</v>
+        <v>3311</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>4001</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="C62" t="s">
+        <v>489</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>999</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>1381</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>1960</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>3655</v>
+      </c>
+      <c r="J62" s="18" t="s">
+        <v>2300</v>
+      </c>
+      <c r="K62" s="18" t="s">
+        <v>2965</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>3312</v>
+      </c>
+      <c r="M62" s="33" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A63" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>482</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>484</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E63" s="18" t="s">
         <v>1001</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>1002</v>
       </c>
-      <c r="G62" s="8" t="s">
+      <c r="G63" s="8" t="s">
         <v>1382</v>
       </c>
-      <c r="H62" s="21" t="s">
+      <c r="H63" s="21" t="s">
         <v>1961</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I63" s="18" t="s">
         <v>3656</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J63" s="18" t="s">
         <v>2301</v>
       </c>
-      <c r="K62" s="18" t="s">
+      <c r="K63" s="18" t="s">
         <v>2966</v>
       </c>
-      <c r="L62" s="18" t="s">
+      <c r="L63" s="18" t="s">
         <v>3313</v>
       </c>
-      <c r="M62" s="33" t="s">
+      <c r="M63" s="33" t="s">
         <v>4003</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A63" t="s">
+    <row r="64" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A64" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B64" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>58</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>647</v>
       </c>
-      <c r="E63" s="18" t="s">
+      <c r="E64" s="18" t="s">
         <v>1003</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>1004</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G64" s="8" t="s">
         <v>1383</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H64" s="21" t="s">
         <v>1962</v>
       </c>
-      <c r="I63" s="18" t="s">
+      <c r="I64" s="18" t="s">
         <v>3657</v>
       </c>
-      <c r="J63" s="18" t="s">
+      <c r="J64" s="18" t="s">
         <v>2302</v>
       </c>
-      <c r="K63" s="18" t="s">
+      <c r="K64" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="L63" s="18" t="s">
+      <c r="L64" s="18" t="s">
         <v>3314</v>
       </c>
-      <c r="M63" s="33" t="s">
+      <c r="M64" s="33" t="s">
         <v>4004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A64" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C64" t="s">
-        <v>155</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>648</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1005</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>1384</v>
-      </c>
-      <c r="H64" s="21" t="s">
-        <v>1963</v>
-      </c>
-      <c r="I64" s="18" t="s">
-        <v>3658</v>
-      </c>
-      <c r="J64" s="18" t="s">
-        <v>2303</v>
-      </c>
-      <c r="K64" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="L64" s="18" t="s">
-        <v>3315</v>
-      </c>
-      <c r="M64" s="36" t="s">
-        <v>4005</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F65" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>1384</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="I65" s="18" t="s">
         <v>3658</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="K65" s="18" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>3316</v>
+        <v>3315</v>
       </c>
       <c r="M65" s="36" t="s">
         <v>4005</v>
@@ -16791,128 +16833,185 @@
     </row>
     <row r="66" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>486</v>
+        <v>106</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>485</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>487</v>
+        <v>105</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F66" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="K66" s="18" t="s">
-        <v>2967</v>
+        <v>104</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>3317</v>
-      </c>
-      <c r="M66" s="33" t="s">
-        <v>4006</v>
+        <v>3316</v>
+      </c>
+      <c r="M66" s="36" t="s">
+        <v>4005</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>36</v>
+        <v>486</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>37</v>
+        <v>485</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>487</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>38</v>
+        <v>1007</v>
       </c>
       <c r="F67" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>2968</v>
+        <v>3659</v>
       </c>
       <c r="J67" s="18" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="K67" s="18" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>3318</v>
+        <v>3317</v>
       </c>
       <c r="M67" s="33" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>1855</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1854</v>
+        <v>36</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>1856</v>
+        <v>38</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>1857</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>1858</v>
+        <v>600</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>1386</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>1966</v>
+      </c>
+      <c r="I68" s="18" t="s">
+        <v>2968</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>2306</v>
+      </c>
+      <c r="K68" s="18" t="s">
+        <v>2968</v>
+      </c>
+      <c r="L68" s="18" t="s">
+        <v>3318</v>
       </c>
       <c r="M68" s="33" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>1900</v>
+        <v>1855</v>
       </c>
       <c r="B69" t="s">
-        <v>1901</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="M69" s="35" t="s">
-        <v>4009</v>
+        <v>1854</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>1857</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>1858</v>
+      </c>
+      <c r="M69" s="33" t="s">
+        <v>4008</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="B70" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="D70" s="27"/>
       <c r="M70" s="35" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="3" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D71" s="27"/>
+      <c r="M71" s="35" t="s">
         <v>4010</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A72" s="3" t="s">
+        <v>4349</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A73" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4352</v>
       </c>
     </row>
   </sheetData>
@@ -16928,8 +17027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -18347,15 +18446,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -19546,6 +19645,22 @@
       </c>
       <c r="M30" s="33" t="s">
         <v>4289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>4353</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>4355</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>4356</v>
       </c>
     </row>
   </sheetData>
@@ -24360,16 +24475,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="37" style="4" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" customWidth="1"/>
     <col min="5" max="5" width="7" style="4" customWidth="1"/>
@@ -25968,6 +26083,54 @@
         <v>4108</v>
       </c>
     </row>
+    <row r="42" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="4" t="s">
+        <v>4337</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="4" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>4339</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>4340</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="4" t="s">
+        <v>4341</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="4" t="s">
+        <v>4342</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>4348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -25978,8 +26141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>